<commit_message>
Atualização de aba de diagnóstico no PCTI
</commit_message>
<xml_diff>
--- a/Arquivos Externos/Controle CTI_QRD.xlsx
+++ b/Arquivos Externos/Controle CTI_QRD.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelso\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{74D7E0EE-8ED5-4ADD-BB0F-DA27CD835A2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23760" windowHeight="9795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23760" windowHeight="9795"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de ação" sheetId="1" r:id="rId1"/>
-    <sheet name="Cronograma BI QRD" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagnóstico detalhado" sheetId="3" r:id="rId2"/>
+    <sheet name="Cronograma BI QRD" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plano de ação'!$A$6:$M$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Cronograma BI QRD'!$A$2:$I$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plano de ação'!$A$6:$M$38</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="196">
   <si>
     <t>Item</t>
   </si>
@@ -150,9 +146,6 @@
   </si>
   <si>
     <t>Luis</t>
-  </si>
-  <si>
-    <t>Entrega com muito atraso</t>
   </si>
   <si>
     <t>Impactos Principais</t>
@@ -452,82 +445,214 @@
     <t>Usuários impedidos de trabalhar com o novo sistema</t>
   </si>
   <si>
-    <t>01/08/18 - Foi liberado 30/07/18 será avaliado pela equipe.
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>01/08/18 - Entendimento sobre Stage como banco de apoio e Interface Pública
+27/07/18 - Modelo de dados entregue pela equipe de BI e sob avaliação da equipe PSV.
+24/07/18 - O modelo foi solicitado novamente em reunião com equipe de BI e TI QRD, fundamental para conclusão do módulo de SLA
+03/07/18 - Foi definido em reunião com equipes de TI que a base de dados origem para Interface pública será a Stage 1, e portanto foi solicitado novamente o Diagrama para avaliação da TI PSV</t>
+  </si>
+  <si>
+    <t>01/08/18 - Relatórios serão controlados pelo painel da CTI, como pequenos projetos</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será discutido com equipe.</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será criado um resumo sobre dados de biometria e problemas associados</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será feita revisão dos dados do extrato, em comparação com base operacional</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será criado um módulo específico no Jira, direcionado para a responsável pelo controle de acesso, sem contabilização para SLA, mas com acompanhamento do tempo de resposta</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será discutido com Infra até 03/08
+27/07/18 - Sem retorno, em mail enviado para toda a liderança da QRD.
+23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento, fundamental para conclusão do módulo de SLA
+03/07/18 - Definição de uma cópia da Stage 1 com acesso direto à banco de dados via VPN</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será mudado no fluxo Jira, com mudança para "Aguardando solicitante" somente quando a função validar for executada pela equipe de suporte QRD
+24/07/18 - Tratado em reunião com André Machado e Denis, será avaliado para novas ocorrências</t>
+  </si>
+  <si>
+    <t>01/08/18 - Ação apresentada para TI QRD, conforme conversado com André Machado
+24/07/18 - Ficou definido que a resposta automatica será mantida, mas será avaliado pela equipe PSV a diferença entre esta e a efetiva primeira resposta enviada pelo técnico na avaliação inicial do chamado após abertura. Se o tempo for muito elevado, a resposta automática deve ser reavaliada</t>
+  </si>
+  <si>
+    <t>01/08/18 - Será apresentado por Tipo e Criticidade.</t>
+  </si>
+  <si>
+    <t>01/08/18 - Previsto para próxima entrega (Relatórios do Edital)
+23/07/18 - Item foi cobrado em mail para André Machado, com previsão de aplicação a partir de agosto</t>
+  </si>
+  <si>
+    <t>01/08/18 - Citado, será tratado com evidências já enviadas pelo André
+13/07/18 - Divergências apresentadas na reunião de fechamento de SLA de junho, com algumas mudanças justificadas. Todos os meses serão calculados retroativamente pelo módulo de SLA Planserv</t>
+  </si>
+  <si>
+    <t>Totais referentes a contas</t>
+  </si>
+  <si>
+    <t>Ocorrências de guias</t>
+  </si>
+  <si>
+    <t>Nomeclatura de itens no Power BI</t>
+  </si>
+  <si>
+    <t>Valores de Grupos, Subgrupos e Grupo Planserv</t>
+  </si>
+  <si>
+    <t>Número total de beneficiários</t>
+  </si>
+  <si>
+    <t>Ausência de especialidade para itens da tabela</t>
+  </si>
+  <si>
+    <t>Ausência de classificação de liminar em contas</t>
+  </si>
+  <si>
+    <t>Valores não são conferidos, e não batem com totais gerais de pagamento</t>
+  </si>
+  <si>
+    <t>Inconsistências devido a problemas frequentes em cargas (defazagem de dados)</t>
+  </si>
+  <si>
+    <t>Informações imcompletas, com muitos itens sem classificação</t>
+  </si>
+  <si>
+    <t>Informações distintas em relação ao módulo de cadastro, módulo de AIS e lista de beneficiários para medição de SLA</t>
+  </si>
+  <si>
+    <t>Atualmente o sistema não relaciona uma especialidade para cada item da tabela, limitando a análise</t>
+  </si>
+  <si>
+    <t>As informações de liminar presentes em autorização ainda não foram correlacionadas a conta, para avaliação de custos</t>
+  </si>
+  <si>
+    <t>Pastas e campos apresentam nome original do banco de dados</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>DW</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
+    <t>Operacional</t>
+  </si>
+  <si>
+    <t>Resolução</t>
+  </si>
+  <si>
+    <t>Item sendo tratado com chamados e também será alvo do ID 3</t>
+  </si>
+  <si>
+    <t>Item sendo tratado como foco do ID 3 do painel de controle (Análise de Valores carregados no BI  )</t>
+  </si>
+  <si>
+    <t>Não é possível avaliar valores de recurso, separar glosa técnica de glosa edital ou glosa 358</t>
+  </si>
+  <si>
+    <t>Campos iniciais previsão somente valor liberado, glosado e cancelado, foi adicionado valor em analise, porém conforme demonstrado pela dificuldade em extração de dados do passivo da glosa edital, uma mudança no lançamentos por prestador é necessária para posterior consolidação no BI</t>
+  </si>
+  <si>
+    <t>Valores divergentes em cada ponto de visualização, um trabalho deve ser realizado diretamente na base do cadastro, funcionalidade de sistema que permita contar o total de beneficiários em qualquer data de referência, este total deve então ser apresentado em todos os outros módulos e no BI</t>
+  </si>
+  <si>
+    <t>Citado em reunião do dia 01/08/18, trabalho reportado como em andamento por Ana Cláudia</t>
+  </si>
+  <si>
+    <t>Campos de valor informado, glosa edital, valor de recurso</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Liminar no painel de contas</t>
+  </si>
+  <si>
+    <t>Marcação de liminar ainda não foi associada da solicitação para respectiva conta</t>
+  </si>
+  <si>
+    <t>Avaliação de custos referentes a liminar</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>Nomeclatura em paineis do BI</t>
+  </si>
+  <si>
+    <t>Áreas de construção de visões no Power BI apresentam o nome original do banco de dados</t>
+  </si>
+  <si>
+    <t>Usabilidade comprometida</t>
+  </si>
+  <si>
+    <t>09/08/18 - 
+24/07/18 - Citado em reunião, porém não foi atualizado no painel de pendências da equipe de BI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/08/18 - 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/08/18 - 
+01/08/18 - Alinhado para entrega de previsão de conclusão do fluxo e sua apresentação em próxima reunião
+23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento
+03/07/18 - Devido ao grande número de inconsistências e dados nulos já identificados no BI, foi solicitado formalização do fluxo de conferência de dados </t>
+  </si>
+  <si>
+    <t>09/08/18 - 
+01/08/18 - Foi liberado 30/07/18 será avaliado pela equipe.
 27/01/18 - PRevisão de entrega somente em 17/08, será feito novo alinamento em 31/07 para entendimento das dificuldades técnicas.
 06/07/18 - Foi realizada tentativa de envio do arquivo como alternativa ao acesso web pelo módulo analítico, sem sucesso
 04/07/18 - Formalizado por André Machado em resumo sobre reuniões realizadas em 03 e 04/07. Foi sinalizado por Raniere necessidade de intervenção da TI QRD para que o painel fosse disponibilizado, com previsão de produção na semana de 09 a 13/07, porém entrega ainda não foi realizada até o momento.</t>
   </si>
   <si>
-    <t>01/08/18 - Apontamento dos itens que podem ser quitados pelos construtores para prototipação. Será avaliado pela equipe de BI QRD o que já existe em paineis prontos, e a próxima reunião tratará exclusivamente deste item.
+    <t>09/08/18 - 
+01/08/18 - Apontamento dos itens que podem ser quitados pelos construtores para prototipação. Será avaliado pela equipe de BI QRD o que já existe em paineis prontos, e a próxima reunião tratará exclusivamente deste item.
 23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela equipe de BI QRD até o momento
 19/06/18 - Retorno do PSV com ajustes e aprovação para especificação enviada
 08/06/18 - Envio de especificação sobre levantamento pela QRD
 30/05/18 - Reunião geral para demonstração dos relatórios, alterada para levantamento detalhado com cada área de negócio, pois relatórios não se encontravam prontos</t>
   </si>
   <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>01/08/18 - Entendimento sobre Stage como banco de apoio e Interface Pública
-27/07/18 - Modelo de dados entregue pela equipe de BI e sob avaliação da equipe PSV.
-24/07/18 - O modelo foi solicitado novamente em reunião com equipe de BI e TI QRD, fundamental para conclusão do módulo de SLA
-03/07/18 - Foi definido em reunião com equipes de TI que a base de dados origem para Interface pública será a Stage 1, e portanto foi solicitado novamente o Diagrama para avaliação da TI PSV</t>
-  </si>
-  <si>
-    <t>01/08/18 - Relatórios serão controlados pelo painel da CTI, como pequenos projetos</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será discutido com equipe.</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será criado um resumo sobre dados de biometria e problemas associados</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será feita revisão dos dados do extrato, em comparação com base operacional</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será criado um módulo específico no Jira, direcionado para a responsável pelo controle de acesso, sem contabilização para SLA, mas com acompanhamento do tempo de resposta</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será discutido com Infra até 03/08
-27/07/18 - Sem retorno, em mail enviado para toda a liderança da QRD.
-23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento, fundamental para conclusão do módulo de SLA
-03/07/18 - Definição de uma cópia da Stage 1 com acesso direto à banco de dados via VPN</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será mudado no fluxo Jira, com mudança para "Aguardando solicitante" somente quando a função validar for executada pela equipe de suporte QRD
-24/07/18 - Tratado em reunião com André Machado e Denis, será avaliado para novas ocorrências</t>
-  </si>
-  <si>
-    <t>01/08/18 - Ação apresentada para TI QRD, conforme conversado com André Machado
-24/07/18 - Ficou definido que a resposta automatica será mantida, mas será avaliado pela equipe PSV a diferença entre esta e a efetiva primeira resposta enviada pelo técnico na avaliação inicial do chamado após abertura. Se o tempo for muito elevado, a resposta automática deve ser reavaliada</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será apresentado por Tipo e Criticidade.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01/08/18 - Alinhado para entrega de previsão de conclusão do fluxo e sua apresentação em próxima reunião
-23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento
-03/07/18 - Devido ao grande número de inconsistências e dados nulos já identificados no BI, foi solicitado formalização do fluxo de conferência de dados </t>
-  </si>
-  <si>
-    <t>01/08/18 - Próxima reunião em 09/08/18 14:00, com tema principal de Relatórios do Edital
+    <t>09/08/18 - 
+01/08/18 - Próxima reunião em 09/08/18 14:00, com tema principal de Relatórios do Edital
 23/07/18 -Primeira reunião realizada, com segunda reunião agendada para 31/07/18</t>
   </si>
   <si>
-    <t>01/08/18 - Previsto para próxima entrega (Relatórios do Edital)
-23/07/18 - Item foi cobrado em mail para André Machado, com previsão de aplicação a partir de agosto</t>
-  </si>
-  <si>
-    <t>01/08/18 - Citado, será tratado com evidências já enviadas pelo André
-13/07/18 - Divergências apresentadas na reunião de fechamento de SLA de junho, com algumas mudanças justificadas. Todos os meses serão calculados retroativamente pelo módulo de SLA Planserv</t>
+    <t>Evidência/Exemplo</t>
+  </si>
+  <si>
+    <t>Tratado em reunião do dia 01/08/18, está sendo conduzida revisão e foi priorizado por André Machado. Não existem mais valores nulos, porém deve ser avaliado pela área técnica quanto ao conteúdo.</t>
+  </si>
+  <si>
+    <t>Ainda não disponível</t>
+  </si>
+  <si>
+    <t>Tratado em reunião do dia 24/07/18, não consta no cronograma atualizado da equipe de BI. ID 18 no painel.</t>
+  </si>
+  <si>
+    <t>Padrão demonstrado pelo BI enviado durante transição, deve ser aplicado em todos os paineis de construção. ID 19 no painel.</t>
+  </si>
+  <si>
+    <t>Detalhamento de Inconsistências/Pendências encontradas na Base de Suporte a Decisão</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,8 +730,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +796,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,7 +1020,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -992,6 +1154,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1023,7 +1219,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1031,7 +1227,7 @@
         <xdr:cNvPr id="1025" name="AutoShape 1" descr="Resultado de imagem para planserv">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1070,7 +1266,7 @@
         <xdr:cNvPr id="1027" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1101,10 +1297,255 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3551230</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1657350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9715501" y="704850"/>
+          <a:ext cx="3236904" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3409950</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1467037</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2052" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9829800" y="2457451"/>
+          <a:ext cx="2981325" cy="1352736"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3571875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1565090</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2054" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9801225" y="4181475"/>
+          <a:ext cx="3171825" cy="1450790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3048000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2028437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2056" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10201275" y="11715751"/>
+          <a:ext cx="2247900" cy="1876036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3590925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1116666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2058" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9648825" y="8020051"/>
+          <a:ext cx="3343275" cy="1040465"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1228726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1571625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2219794</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2060" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9648825" y="9172576"/>
+          <a:ext cx="1323975" cy="991068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1142,9 +1583,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1176,27 +1617,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1228,27 +1651,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1421,14 +1826,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -1443,8 +1849,8 @@
     <col min="13" max="13" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1">
       <c r="A2" s="44"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
@@ -1463,7 +1869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="22.5" customHeight="1">
       <c r="A3" s="45"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
@@ -1482,7 +1888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" thickBot="1">
       <c r="A4" s="46"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -1501,7 +1907,7 @@
       <c r="L4" s="49"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="31.5">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1521,10 +1927,10 @@
         <v>3</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>4</v>
@@ -1542,7 +1948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="210" hidden="1">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -1556,13 +1962,13 @@
         <v>12</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="7" t="s">
@@ -1571,15 +1977,15 @@
       <c r="J7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="26">
-        <v>43321</v>
+      <c r="K7" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="165">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -1599,7 +2005,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="7" t="s">
@@ -1608,26 +2014,26 @@
       <c r="J8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="57">
         <v>43315</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="165" hidden="1">
       <c r="A9" s="7">
         <v>3</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>25</v>
@@ -1636,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="7" t="s">
@@ -1649,11 +2055,11 @@
         <v>43321</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="105" hidden="1">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -1673,7 +2079,7 @@
         <v>30</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="7" t="s">
@@ -1686,31 +2092,31 @@
         <v>43321</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="270" hidden="1">
       <c r="A11" s="7">
         <v>5</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>114</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="7" t="s">
@@ -1719,35 +2125,35 @@
       <c r="J11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="26">
-        <v>43321</v>
+      <c r="K11" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="285" hidden="1">
       <c r="A12" s="7">
         <v>6</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>52</v>
-      </c>
       <c r="D12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>115</v>
+        <v>53</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="7" t="s">
@@ -1760,31 +2166,31 @@
         <v>43321</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="75" hidden="1">
       <c r="A13" s="7">
         <v>7</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="7" t="s">
@@ -1793,15 +2199,15 @@
       <c r="J13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="26">
-        <v>43321</v>
+      <c r="K13" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="105" hidden="1">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -1821,7 +2227,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="7" t="s">
@@ -1834,11 +2240,11 @@
         <v>37</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="105" hidden="1">
       <c r="A15" s="7">
         <v>9</v>
       </c>
@@ -1858,7 +2264,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="7" t="s">
@@ -1871,341 +2277,381 @@
         <v>37</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="90" hidden="1">
       <c r="A16" s="7">
         <v>10</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="K16" s="26">
-        <v>43321</v>
+        <v>105</v>
+      </c>
+      <c r="K16" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="120" hidden="1">
       <c r="A17" s="7">
         <v>11</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="K17" s="26">
-        <v>43321</v>
+        <v>109</v>
+      </c>
+      <c r="K17" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="45" hidden="1">
       <c r="A18" s="7">
         <v>12</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="K18" s="26">
-        <v>43321</v>
+        <v>113</v>
+      </c>
+      <c r="K18" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="60" hidden="1">
       <c r="A19" s="7">
         <v>13</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="D19" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="15" t="s">
         <v>118</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>119</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="K19" s="26">
-        <v>43321</v>
+        <v>105</v>
+      </c>
+      <c r="K19" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L19" s="43" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="60" hidden="1">
       <c r="A20" s="7">
         <v>14</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="18" t="s">
         <v>133</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>134</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="K20" s="26">
-        <v>43321</v>
+        <v>109</v>
+      </c>
+      <c r="K20" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="75" hidden="1">
       <c r="A21" s="7">
         <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E21" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="K21" s="26">
-        <v>43321</v>
+        <v>123</v>
+      </c>
+      <c r="K21" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L21" s="43" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M21" s="11"/>
     </row>
-    <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="60" hidden="1">
       <c r="A22" s="7">
         <v>16</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="K22" s="26">
-        <v>43321</v>
+        <v>126</v>
+      </c>
+      <c r="K22" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="60">
       <c r="A23" s="7">
         <v>17</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="K23" s="26">
-        <v>43321</v>
+        <v>113</v>
+      </c>
+      <c r="K23" s="57">
+        <v>43315</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="60" hidden="1">
       <c r="A24" s="7">
         <v>18</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="16"/>
+      <c r="B24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>179</v>
+      </c>
       <c r="H24" s="16"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="11"/>
+      <c r="I24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="26">
+        <v>43321</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="M24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="45" hidden="1">
       <c r="A25" s="7">
         <v>19</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="16"/>
+      <c r="B25" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>183</v>
+      </c>
       <c r="H25" s="16"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="11"/>
+      <c r="I25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="26">
+        <v>43321</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="30.75" hidden="1" customHeight="1">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -2222,8 +2668,218 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
     </row>
+    <row r="27" spans="1:13" hidden="1">
+      <c r="A27" s="7">
+        <v>21</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" hidden="1">
+      <c r="A28" s="7">
+        <v>22</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" hidden="1">
+      <c r="A29" s="7">
+        <v>23</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" hidden="1">
+      <c r="A30" s="7">
+        <v>24</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" hidden="1">
+      <c r="A31" s="7">
+        <v>25</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" hidden="1">
+      <c r="A32" s="7">
+        <v>26</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" hidden="1">
+      <c r="A33" s="7">
+        <v>27</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+    </row>
+    <row r="34" spans="1:13" hidden="1">
+      <c r="A34" s="7">
+        <v>28</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" hidden="1">
+      <c r="A35" s="7">
+        <v>29</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+    </row>
+    <row r="36" spans="1:13" hidden="1">
+      <c r="A36" s="7">
+        <v>30</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" hidden="1">
+      <c r="A37" s="7">
+        <v>31</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" hidden="1">
+      <c r="A38" s="7">
+        <v>32</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A6:M26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:M38">
+    <filterColumn colId="10">
+      <filters>
+        <dateGroupItem year="2018" month="8" day="3" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="L2:L4"/>
@@ -2235,14 +2891,194 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="58" style="19" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" style="61" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="27" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A1" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="61"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="154.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="135.75" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="140.25" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="165">
+      <c r="A7" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="193.5" customHeight="1">
+      <c r="A8" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="60">
+      <c r="A9" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60">
+      <c r="A10" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="174" customHeight="1">
+      <c r="A11" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I236"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.5703125" customWidth="1"/>
@@ -2255,9 +3091,9 @@
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75">
       <c r="A1" s="50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -2268,42 +3104,42 @@
       <c r="H1" s="51"/>
       <c r="I1" s="51"/>
     </row>
-    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="31.5">
       <c r="A2" s="32"/>
       <c r="B2" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="D2" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="E2" s="33" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>59</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="I2" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" hidden="1">
       <c r="A3" s="28">
         <v>1</v>
       </c>
       <c r="B3" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>63</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>64</v>
       </c>
       <c r="D3" s="36">
         <v>43283</v>
@@ -2312,23 +3148,23 @@
         <v>43284</v>
       </c>
       <c r="F3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="29" t="s">
         <v>65</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>66</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="35"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1">
       <c r="A4" s="28">
         <v>2</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="36">
         <v>43283</v>
@@ -2337,23 +3173,23 @@
         <v>43284</v>
       </c>
       <c r="F4" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>65</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>66</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="35"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+    <row r="5" spans="1:9" ht="25.5">
+      <c r="A5" s="63">
         <v>3</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="36">
         <v>43285</v>
@@ -2363,22 +3199,22 @@
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="35"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="63">
+        <v>4</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="35"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
-        <v>4</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>70</v>
-      </c>
       <c r="C6" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="36">
         <v>43286</v>
@@ -2388,20 +3224,20 @@
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="35"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+    <row r="7" spans="1:9">
+      <c r="A7" s="63">
         <v>5</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="36">
         <v>43284</v>
@@ -2411,22 +3247,22 @@
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I7" s="35"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="25.5" hidden="1">
       <c r="A8" s="28">
         <v>6</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="36">
         <v>43287</v>
@@ -2435,23 +3271,23 @@
         <v>43287</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+    <row r="9" spans="1:9" ht="25.5">
+      <c r="A9" s="63">
         <v>7</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="36">
         <v>43305</v>
@@ -2462,19 +3298,19 @@
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" ht="38.25">
+      <c r="A10" s="63">
+        <v>8</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
-        <v>8</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>78</v>
-      </c>
       <c r="C10" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="36">
         <v>43305</v>
@@ -2484,22 +3320,22 @@
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="25.5" hidden="1">
       <c r="A11" s="28">
         <v>9</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="36">
         <v>43271</v>
@@ -2508,23 +3344,23 @@
         <v>43271</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="30"/>
       <c r="I11" s="35"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1">
       <c r="A12" s="28">
         <v>10</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="36">
         <v>43271</v>
@@ -2533,23 +3369,23 @@
         <v>43271</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12" s="30"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+    <row r="13" spans="1:9">
+      <c r="A13" s="63">
         <v>11</v>
       </c>
       <c r="B13" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>83</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>84</v>
       </c>
       <c r="D13" s="36">
         <v>43278</v>
@@ -2558,25 +3394,25 @@
         <v>43315</v>
       </c>
       <c r="F13" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="H13" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="63">
+        <v>12</v>
+      </c>
+      <c r="B14" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
-        <v>12</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>88</v>
-      </c>
       <c r="C14" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="36">
         <v>43290</v>
@@ -2585,23 +3421,23 @@
         <v>43294</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="35"/>
     </row>
-    <row r="15" spans="1:9" ht="153" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+    <row r="15" spans="1:9" ht="153">
+      <c r="A15" s="63">
         <v>13</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="36">
         <v>43297</v>
@@ -2610,25 +3446,25 @@
         <v>43315</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>92</v>
-      </c>
       <c r="I15" s="35"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1">
       <c r="A16" s="28">
         <v>14</v>
       </c>
       <c r="B16" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>94</v>
       </c>
       <c r="D16" s="36">
         <v>43318</v>
@@ -2641,15 +3477,15 @@
       <c r="H16" s="30"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+    <row r="17" spans="1:9" ht="38.25">
+      <c r="A17" s="63">
         <v>15</v>
       </c>
       <c r="B17" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>95</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>96</v>
       </c>
       <c r="D17" s="36">
         <v>43280</v>
@@ -2658,28 +3494,30 @@
         <v>43313</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17" s="35"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="28"/>
       <c r="B18" s="34"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
+      <c r="F18" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="G18" s="29"/>
       <c r="H18" s="30"/>
       <c r="I18" s="35"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="28"/>
       <c r="B19" s="34"/>
       <c r="C19" s="28"/>
@@ -2690,7 +3528,7 @@
       <c r="H19" s="30"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="28"/>
       <c r="B20" s="34"/>
       <c r="C20" s="28"/>
@@ -2701,7 +3539,7 @@
       <c r="H20" s="30"/>
       <c r="I20" s="35"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="28"/>
       <c r="B21" s="34"/>
       <c r="C21" s="28"/>
@@ -2712,7 +3550,7 @@
       <c r="H21" s="30"/>
       <c r="I21" s="35"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="28"/>
       <c r="B22" s="34"/>
       <c r="C22" s="28"/>
@@ -2723,7 +3561,7 @@
       <c r="H22" s="30"/>
       <c r="I22" s="35"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="28"/>
       <c r="B23" s="34"/>
       <c r="C23" s="28"/>
@@ -2734,7 +3572,7 @@
       <c r="H23" s="30"/>
       <c r="I23" s="35"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="28"/>
       <c r="B24" s="34"/>
       <c r="C24" s="28"/>
@@ -2745,7 +3583,7 @@
       <c r="H24" s="30"/>
       <c r="I24" s="35"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="28"/>
       <c r="B25" s="34"/>
       <c r="C25" s="28"/>
@@ -2756,7 +3594,7 @@
       <c r="H25" s="30"/>
       <c r="I25" s="35"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="28"/>
       <c r="B26" s="34"/>
       <c r="C26" s="28"/>
@@ -2767,7 +3605,7 @@
       <c r="H26" s="30"/>
       <c r="I26" s="35"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -2778,7 +3616,7 @@
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="27"/>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -2789,7 +3627,7 @@
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="27"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -2800,7 +3638,7 @@
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="27"/>
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
@@ -2811,7 +3649,7 @@
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="27"/>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -2822,7 +3660,7 @@
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
@@ -2833,7 +3671,7 @@
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9">
       <c r="A225" s="27"/>
       <c r="B225" s="27"/>
       <c r="C225" s="27"/>
@@ -2844,7 +3682,7 @@
       <c r="H225" s="27"/>
       <c r="I225" s="27"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9">
       <c r="A226" s="27"/>
       <c r="B226" s="27"/>
       <c r="C226" s="27"/>
@@ -2855,7 +3693,7 @@
       <c r="H226" s="27"/>
       <c r="I226" s="27"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9">
       <c r="A227" s="27"/>
       <c r="B227" s="27"/>
       <c r="C227" s="27"/>
@@ -2866,7 +3704,7 @@
       <c r="H227" s="27"/>
       <c r="I227" s="27"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9">
       <c r="A228" s="27"/>
       <c r="B228" s="27"/>
       <c r="C228" s="27"/>
@@ -2877,7 +3715,7 @@
       <c r="H228" s="27"/>
       <c r="I228" s="27"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9">
       <c r="A229" s="27"/>
       <c r="B229" s="27"/>
       <c r="C229" s="27"/>
@@ -2888,7 +3726,7 @@
       <c r="H229" s="27"/>
       <c r="I229" s="27"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9">
       <c r="A230" s="27"/>
       <c r="B230" s="27"/>
       <c r="C230" s="27"/>
@@ -2899,7 +3737,7 @@
       <c r="H230" s="27"/>
       <c r="I230" s="27"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9">
       <c r="A231" s="27"/>
       <c r="B231" s="27"/>
       <c r="C231" s="27"/>
@@ -2910,7 +3748,7 @@
       <c r="H231" s="27"/>
       <c r="I231" s="27"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9">
       <c r="A232" s="27"/>
       <c r="B232" s="27"/>
       <c r="C232" s="27"/>
@@ -2921,7 +3759,7 @@
       <c r="H232" s="27"/>
       <c r="I232" s="27"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9">
       <c r="A233" s="27"/>
       <c r="B233" s="27"/>
       <c r="C233" s="27"/>
@@ -2932,7 +3770,7 @@
       <c r="H233" s="27"/>
       <c r="I233" s="27"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9">
       <c r="A234" s="27"/>
       <c r="B234" s="27"/>
       <c r="C234" s="27"/>
@@ -2943,7 +3781,7 @@
       <c r="H234" s="27"/>
       <c r="I234" s="27"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9">
       <c r="A235" s="27"/>
       <c r="B235" s="27"/>
       <c r="C235" s="27"/>
@@ -2954,7 +3792,7 @@
       <c r="H235" s="27"/>
       <c r="I235" s="27"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9">
       <c r="A236" s="27"/>
       <c r="B236" s="27"/>
       <c r="C236" s="27"/>
@@ -2966,6 +3804,21 @@
       <c r="I236" s="27"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:I18">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <dateGroupItem year="2018" month="6" dateTimeGrouping="month"/>
+        <dateGroupItem year="2018" month="7" dateTimeGrouping="month"/>
+        <dateGroupItem year="2018" month="8" day="1" dateTimeGrouping="day"/>
+        <dateGroupItem year="2018" month="8" day="3" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="Homologação"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Alterações de André Mendes
</commit_message>
<xml_diff>
--- a/Arquivos Externos/Controle CTI_QRD.xlsx
+++ b/Arquivos Externos/Controle CTI_QRD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="199">
   <si>
     <t>Item</t>
   </si>
@@ -460,32 +460,16 @@
     <t>01/08/18 - Será discutido com equipe.</t>
   </si>
   <si>
-    <t>01/08/18 - Será criado um resumo sobre dados de biometria e problemas associados</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será feita revisão dos dados do extrato, em comparação com base operacional</t>
-  </si>
-  <si>
-    <t>01/08/18 - Será criado um módulo específico no Jira, direcionado para a responsável pelo controle de acesso, sem contabilização para SLA, mas com acompanhamento do tempo de resposta</t>
-  </si>
-  <si>
     <t>01/08/18 - Será discutido com Infra até 03/08
 27/07/18 - Sem retorno, em mail enviado para toda a liderança da QRD.
 23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento, fundamental para conclusão do módulo de SLA
 03/07/18 - Definição de uma cópia da Stage 1 com acesso direto à banco de dados via VPN</t>
   </si>
   <si>
-    <t>01/08/18 - Será mudado no fluxo Jira, com mudança para "Aguardando solicitante" somente quando a função validar for executada pela equipe de suporte QRD
-24/07/18 - Tratado em reunião com André Machado e Denis, será avaliado para novas ocorrências</t>
-  </si>
-  <si>
     <t>01/08/18 - Ação apresentada para TI QRD, conforme conversado com André Machado
 24/07/18 - Ficou definido que a resposta automatica será mantida, mas será avaliado pela equipe PSV a diferença entre esta e a efetiva primeira resposta enviada pelo técnico na avaliação inicial do chamado após abertura. Se o tempo for muito elevado, a resposta automática deve ser reavaliada</t>
   </si>
   <si>
-    <t>01/08/18 - Será apresentado por Tipo e Criticidade.</t>
-  </si>
-  <si>
     <t>01/08/18 - Previsto para próxima entrega (Relatórios do Edital)
 23/07/18 - Item foi cobrado em mail para André Machado, com previsão de aplicação a partir de agosto</t>
   </si>
@@ -570,9 +554,6 @@
   </si>
   <si>
     <t>Campos de valor informado, glosa edital, valor de recurso</t>
-  </si>
-  <si>
-    <t>Em andamento</t>
   </si>
   <si>
     <t>Liminar no painel de contas</t>
@@ -655,6 +636,30 @@
   </si>
   <si>
     <t>Padrão demonstrado pelo BI enviado durante transição, deve ser aplicado em todos os paineis de construção. ID 19 no painel</t>
+  </si>
+  <si>
+    <t>03/08/18 - Criado novo projeto no Jira (ACESSOS) consolidando chamados de acesso.
+01/08/18 - Será criado um módulo específico no Jira, direcionado para a responsável pelo controle de acesso, sem contabilização para SLA, mas com acompanhamento do tempo de resposta</t>
+  </si>
+  <si>
+    <t>03/08/18 - Removida a automação que muda o status do chamado quando o atendente comenta. A alteração será manual.
+01/08/18 - Será mudado no fluxo Jira, com mudança para "Aguardando solicitante" somente quando a função validar for executada pela equipe de suporte QRD
+24/07/18 - Tratado em reunião com André Machado e Denis, será avaliado para novas ocorrências</t>
+  </si>
+  <si>
+    <t>03/08/18 - Será tratado diretamente com André Duarte em reunião presencial.
+01/08/18 - Será apresentado por Tipo e Criticidade.</t>
+  </si>
+  <si>
+    <t>Aguardando deliberação</t>
+  </si>
+  <si>
+    <t>03/08/18 - Relatório em elaboração por Denis, informado por André Duarte.
+01/08/18 - Será criado um resumo sobre dados de biometria e problemas associados</t>
+  </si>
+  <si>
+    <t>03/08/18 - Cálculo de coparticipação realizado no dia 02/08 e os dados estarão disponíveis no extrato do beneficiário.
+01/08/18 - Será feita revisão dos dados do extrato, em comparação com base operacional</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1233,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1236,7 +1241,7 @@
         <xdr:cNvPr id="1025" name="AutoShape 1" descr="Resultado de imagem para planserv">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1275,7 +1280,7 @@
         <xdr:cNvPr id="1027" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1876,7 +1881,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -1997,7 +2001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="210" hidden="1">
+    <row r="7" spans="1:13" ht="210">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -2027,7 +2031,7 @@
         <v>15</v>
       </c>
       <c r="K7" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>138</v>
@@ -2067,11 +2071,11 @@
         <v>43315</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="165" hidden="1">
+    <row r="9" spans="1:13" ht="165">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -2104,11 +2108,11 @@
         <v>43321</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="105" hidden="1">
+    <row r="10" spans="1:13" ht="105">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -2141,11 +2145,11 @@
         <v>43321</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="270" hidden="1">
+    <row r="11" spans="1:13" ht="270">
       <c r="A11" s="7">
         <v>5</v>
       </c>
@@ -2175,14 +2179,14 @@
         <v>26</v>
       </c>
       <c r="K11" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" ht="285" hidden="1">
+    <row r="12" spans="1:13" ht="285">
       <c r="A12" s="7">
         <v>6</v>
       </c>
@@ -2215,11 +2219,11 @@
         <v>43321</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" ht="75" hidden="1">
+    <row r="13" spans="1:13" ht="75">
       <c r="A13" s="7">
         <v>7</v>
       </c>
@@ -2249,14 +2253,14 @@
         <v>26</v>
       </c>
       <c r="K13" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" ht="105" hidden="1">
+    <row r="14" spans="1:13" ht="105">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -2289,11 +2293,11 @@
         <v>37</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="1:13" ht="105" hidden="1">
+    <row r="15" spans="1:13" ht="105">
       <c r="A15" s="7">
         <v>9</v>
       </c>
@@ -2326,11 +2330,11 @@
         <v>37</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" ht="90" hidden="1">
+    <row r="16" spans="1:13" ht="150">
       <c r="A16" s="7">
         <v>10</v>
       </c>
@@ -2343,8 +2347,8 @@
       <c r="D16" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>106</v>
+      <c r="E16" s="17" t="s">
+        <v>114</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>30</v>
@@ -2360,14 +2364,14 @@
         <v>105</v>
       </c>
       <c r="K16" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13" ht="120" hidden="1">
+    <row r="17" spans="1:13" ht="120">
       <c r="A17" s="7">
         <v>11</v>
       </c>
@@ -2397,14 +2401,14 @@
         <v>109</v>
       </c>
       <c r="K17" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" ht="45" hidden="1">
+    <row r="18" spans="1:13" ht="60">
       <c r="A18" s="7">
         <v>12</v>
       </c>
@@ -2417,8 +2421,8 @@
       <c r="D18" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>176</v>
+      <c r="E18" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>30</v>
@@ -2433,15 +2437,15 @@
       <c r="J18" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="48" t="s">
-        <v>180</v>
+      <c r="K18" s="26">
+        <v>43321</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" ht="60" hidden="1">
+    <row r="19" spans="1:13" ht="60">
       <c r="A19" s="7">
         <v>13</v>
       </c>
@@ -2471,14 +2475,14 @@
         <v>105</v>
       </c>
       <c r="K19" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L19" s="43" t="s">
         <v>139</v>
       </c>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" ht="60" hidden="1">
+    <row r="20" spans="1:13" ht="60">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -2508,14 +2512,14 @@
         <v>109</v>
       </c>
       <c r="K20" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L20" s="43" t="s">
         <v>140</v>
       </c>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" ht="75" hidden="1">
+    <row r="21" spans="1:13" ht="75">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -2545,14 +2549,14 @@
         <v>123</v>
       </c>
       <c r="K21" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L21" s="43" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="M21" s="11"/>
     </row>
-    <row r="22" spans="1:13" ht="60" hidden="1">
+    <row r="22" spans="1:13" ht="105" customHeight="1">
       <c r="A22" s="7">
         <v>16</v>
       </c>
@@ -2582,14 +2586,14 @@
         <v>126</v>
       </c>
       <c r="K22" s="48" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13" ht="60">
+    <row r="23" spans="1:13" ht="105">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -2603,7 +2607,7 @@
         <v>135</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>30</v>
@@ -2622,22 +2626,22 @@
         <v>43315</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:13" ht="60" hidden="1">
+    <row r="24" spans="1:13" ht="60">
       <c r="A24" s="7">
         <v>18</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E24" s="46" t="s">
         <v>112</v>
@@ -2646,7 +2650,7 @@
         <v>13</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="7" t="s">
@@ -2659,22 +2663,22 @@
         <v>43321</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="M24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="45" hidden="1">
+    <row r="25" spans="1:13" ht="45">
       <c r="A25" s="7">
         <v>19</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E25" s="46" t="s">
         <v>112</v>
@@ -2683,7 +2687,7 @@
         <v>30</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="7" t="s">
@@ -2696,11 +2700,11 @@
         <v>43321</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" ht="30.75" hidden="1" customHeight="1">
+    <row r="26" spans="1:13" ht="30.75" customHeight="1">
       <c r="A26" s="7">
         <v>20</v>
       </c>
@@ -2717,7 +2721,7 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
     </row>
-    <row r="27" spans="1:13" hidden="1">
+    <row r="27" spans="1:13">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -2734,7 +2738,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row r="28" spans="1:13" hidden="1">
+    <row r="28" spans="1:13">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -2751,7 +2755,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="1:13" hidden="1">
+    <row r="29" spans="1:13">
       <c r="A29" s="7">
         <v>23</v>
       </c>
@@ -2768,7 +2772,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="7">
         <v>24</v>
       </c>
@@ -2785,7 +2789,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" s="7">
         <v>25</v>
       </c>
@@ -2802,7 +2806,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" s="7">
         <v>26</v>
       </c>
@@ -2819,7 +2823,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="1:13" hidden="1">
+    <row r="33" spans="1:13">
       <c r="A33" s="7">
         <v>27</v>
       </c>
@@ -2836,7 +2840,7 @@
       <c r="L33" s="11"/>
       <c r="M33" s="11"/>
     </row>
-    <row r="34" spans="1:13" hidden="1">
+    <row r="34" spans="1:13">
       <c r="A34" s="7">
         <v>28</v>
       </c>
@@ -2853,7 +2857,7 @@
       <c r="L34" s="11"/>
       <c r="M34" s="11"/>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" s="7">
         <v>29</v>
       </c>
@@ -2870,7 +2874,7 @@
       <c r="L35" s="11"/>
       <c r="M35" s="11"/>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" s="7">
         <v>30</v>
       </c>
@@ -2887,7 +2891,7 @@
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
     </row>
-    <row r="37" spans="1:13" hidden="1">
+    <row r="37" spans="1:13">
       <c r="A37" s="7">
         <v>31</v>
       </c>
@@ -2904,7 +2908,7 @@
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" s="7">
         <v>32</v>
       </c>
@@ -2923,11 +2927,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A6:M38">
-    <filterColumn colId="10">
-      <filters>
-        <dateGroupItem year="2018" month="8" day="3" dateTimeGrouping="day"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="10"/>
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A2:A4"/>
@@ -2958,7 +2958,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="27" customFormat="1" ht="42.75" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -2970,156 +2970,156 @@
         <v>0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="154.5" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C4" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>165</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>170</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="135.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="140.25" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="165">
       <c r="A7" s="11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C7" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="51" t="s">
-        <v>172</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="193.5" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" ht="60">
       <c r="A9" s="11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60">
       <c r="A10" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="174" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D11" s="51" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="112.5" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E12" s="7"/>
     </row>

</xml_diff>

<commit_message>
Atualização do item de VPN
</commit_message>
<xml_diff>
--- a/Arquivos Externos/Controle CTI_QRD.xlsx
+++ b/Arquivos Externos/Controle CTI_QRD.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena\Documents\RGitRep\Arquivos Externos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D972BD4-D06A-4686-99C0-399330C9A744}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20280" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="20280" windowHeight="8025"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de ação" sheetId="1" r:id="rId1"/>
@@ -22,12 +16,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Cronograma BI QRD'!$A$2:$I$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Plano de ação'!$A$6:$M$38</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="270">
   <si>
     <t>Item</t>
   </si>
@@ -458,12 +452,6 @@
 03/07/18 - Foi definido em reunião com equipes de TI que a base de dados origem para Interface pública será a Stage 1, e portanto foi solicitado novamente o Diagrama para avaliação da TI PSV</t>
   </si>
   <si>
-    <t>01/08/18 - Será discutido com Infra até 03/08
-27/07/18 - Sem retorno, em mail enviado para toda a liderança da QRD.
-23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento, fundamental para conclusão do módulo de SLA
-03/07/18 - Definição de uma cópia da Stage 1 com acesso direto à banco de dados via VPN</t>
-  </si>
-  <si>
     <t>01/08/18 - Ação apresentada para TI QRD, conforme conversado com André Machado
 24/07/18 - Ficou definido que a resposta automatica será mantida, mas será avaliado pela equipe PSV a diferença entre esta e a efetiva primeira resposta enviada pelo técnico na avaliação inicial do chamado após abertura. Se o tempo for muito elevado, a resposta automática deve ser reavaliada</t>
   </si>
@@ -685,9 +673,6 @@
     <t>Raniere/Bernardo</t>
   </si>
   <si>
-    <t>09/08/18 - Foram identificadas tabelas sem dados atualizados, e também fomos informados que a carga está sendo realizada sob demanda. Em reunião foi definido que a base deve estar espelhada com a STG 1 de produção em D-1, o método poderá ser definido pela equipe técnica da QRD, espelhamento ou cargas simultâneas</t>
-  </si>
-  <si>
     <t>11.4.7.8 Módulo Relatórios</t>
   </si>
   <si>
@@ -884,13 +869,27 @@
   </si>
   <si>
     <t>Atualização de dados da Cópia_STG 1</t>
+  </si>
+  <si>
+    <t>03/08/18 - Acesso liberado conforme previsto, atualmente em avaliação pela TI PSV
+01/08/18 - Será discutido com Infra até 03/08
+27/07/18 - Sem retorno, em mail enviado para toda a liderança da QRD.
+23/07/18 - Item foi cobrado em mail para André Machado, sem retorno pela TI QRD até o momento, fundamental para conclusão do módulo de SLA
+03/07/18 - Definição de uma cópia da Stage 1 com acesso direto à banco de dados via VPN</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>10/08/18 - Reuniões estão sendo conduzidas pelas equipes de TI e BI QRD para ajuste do processo de carga
+09/08/18 - Foram identificadas tabelas sem dados atualizados, e também fomos informados que a carga está sendo realizada sob demanda. Em reunião foi definido que a base deve estar espelhada com a STG 1 de produção em D-1, o método poderá ser definido pela equipe técnica da QRD, espelhamento ou cargas simultâneas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1417,41 +1416,41 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1490,7 +1489,7 @@
         <xdr:cNvPr id="1025" name="AutoShape 1" descr="Resultado de imagem para planserv">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1529,7 +1528,7 @@
         <xdr:cNvPr id="1027" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1580,7 +1579,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1625,7 @@
         <xdr:cNvPr id="2052" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1672,7 +1671,7 @@
         <xdr:cNvPr id="2054" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1718,7 +1717,7 @@
         <xdr:cNvPr id="2056" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1764,7 +1763,7 @@
         <xdr:cNvPr id="2058" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1810,7 +1809,7 @@
         <xdr:cNvPr id="2060" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1856,7 +1855,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1890,7 +1889,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1928,9 +1927,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1962,27 +1961,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2014,27 +1995,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2207,14 +2170,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -2229,9 +2192,9 @@
     <col min="13" max="13" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55"/>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1">
+      <c r="A2" s="59"/>
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
@@ -2244,13 +2207,13 @@
       <c r="I2" s="1"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
-      <c r="L2" s="58"/>
+      <c r="L2" s="62"/>
       <c r="M2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
+    <row r="3" spans="1:13" ht="22.5" customHeight="1">
+      <c r="A3" s="60"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2263,13 +2226,13 @@
       <c r="I3" s="6"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="59"/>
+      <c r="L3" s="63"/>
       <c r="M3" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A4" s="61"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2284,10 +2247,10 @@
       <c r="I4" s="3"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
-      <c r="L4" s="60"/>
+      <c r="L4" s="64"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="31.5">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -2328,7 +2291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="210">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -2358,14 +2321,14 @@
         <v>15</v>
       </c>
       <c r="K7" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>137</v>
       </c>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="210">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -2378,8 +2341,8 @@
       <c r="D8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>19</v>
+      <c r="E8" s="17" t="s">
+        <v>113</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>13</v>
@@ -2394,15 +2357,15 @@
       <c r="J8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="48">
-        <v>43315</v>
+      <c r="K8" s="47" t="s">
+        <v>169</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>138</v>
+        <v>267</v>
       </c>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="180">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -2435,11 +2398,11 @@
         <v>43328</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="105">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -2472,11 +2435,11 @@
         <v>43328</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="270" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="270">
       <c r="A11" s="7">
         <v>5</v>
       </c>
@@ -2506,14 +2469,14 @@
         <v>26</v>
       </c>
       <c r="K11" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" ht="360" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="360">
       <c r="A12" s="7">
         <v>6</v>
       </c>
@@ -2546,11 +2509,11 @@
         <v>43325</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="75">
       <c r="A13" s="7">
         <v>7</v>
       </c>
@@ -2580,14 +2543,14 @@
         <v>26</v>
       </c>
       <c r="K13" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="150">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -2620,11 +2583,11 @@
         <v>37</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="150">
       <c r="A15" s="7">
         <v>9</v>
       </c>
@@ -2657,11 +2620,11 @@
         <v>37</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="150">
       <c r="A16" s="7">
         <v>10</v>
       </c>
@@ -2691,14 +2654,14 @@
         <v>105</v>
       </c>
       <c r="K16" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="120">
       <c r="A17" s="7">
         <v>11</v>
       </c>
@@ -2728,14 +2691,14 @@
         <v>109</v>
       </c>
       <c r="K17" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="165">
       <c r="A18" s="7">
         <v>12</v>
       </c>
@@ -2749,7 +2712,7 @@
         <v>111</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>30</v>
@@ -2765,14 +2728,14 @@
         <v>112</v>
       </c>
       <c r="K18" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="90">
       <c r="A19" s="7">
         <v>13</v>
       </c>
@@ -2805,11 +2768,11 @@
         <v>43328</v>
       </c>
       <c r="L19" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="147.75" customHeight="1">
       <c r="A20" s="7">
         <v>14</v>
       </c>
@@ -2842,11 +2805,11 @@
         <v>43325</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="135">
       <c r="A21" s="7">
         <v>15</v>
       </c>
@@ -2876,14 +2839,14 @@
         <v>122</v>
       </c>
       <c r="K21" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L21" s="43" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M21" s="11"/>
     </row>
-    <row r="22" spans="1:13" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="105" customHeight="1">
       <c r="A22" s="7">
         <v>16</v>
       </c>
@@ -2913,14 +2876,14 @@
         <v>125</v>
       </c>
       <c r="K22" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="105">
       <c r="A23" s="7">
         <v>17</v>
       </c>
@@ -2953,31 +2916,31 @@
         <v>43315</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="90">
       <c r="A24" s="7">
         <v>18</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="7" t="s">
@@ -2990,22 +2953,22 @@
         <v>43328</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="60">
       <c r="A25" s="7">
         <v>19</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>113</v>
@@ -3014,7 +2977,7 @@
         <v>30</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="7" t="s">
@@ -3024,51 +2987,51 @@
         <v>26</v>
       </c>
       <c r="K25" s="47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="142.5" customHeight="1">
       <c r="A26" s="7">
         <v>20</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>192</v>
+        <v>268</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K26" s="26">
         <v>43322</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>202</v>
+        <v>269</v>
       </c>
       <c r="M26" s="11"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="7">
         <v>21</v>
       </c>
@@ -3085,7 +3048,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="7">
         <v>22</v>
       </c>
@@ -3102,7 +3065,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="7">
         <v>23</v>
       </c>
@@ -3119,7 +3082,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="7">
         <v>24</v>
       </c>
@@ -3136,7 +3099,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="7">
         <v>25</v>
       </c>
@@ -3153,7 +3116,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="7">
         <v>26</v>
       </c>
@@ -3170,7 +3133,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="7">
         <v>27</v>
       </c>
@@ -3187,7 +3150,7 @@
       <c r="L33" s="11"/>
       <c r="M33" s="11"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="7">
         <v>28</v>
       </c>
@@ -3204,7 +3167,7 @@
       <c r="L34" s="11"/>
       <c r="M34" s="11"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="7">
         <v>29</v>
       </c>
@@ -3221,7 +3184,7 @@
       <c r="L35" s="11"/>
       <c r="M35" s="11"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="7">
         <v>30</v>
       </c>
@@ -3238,7 +3201,7 @@
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="7">
         <v>31</v>
       </c>
@@ -3255,7 +3218,7 @@
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="7">
         <v>32</v>
       </c>
@@ -3273,7 +3236,7 @@
       <c r="M38" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:M38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:M38"/>
   <mergeCells count="2">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="L2:L4"/>
@@ -3285,487 +3248,487 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E6B3A4-4660-4732-B0B7-3959BA325D5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="27" customWidth="1"/>
     <col min="2" max="2" width="114.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="27" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="68"/>
-    </row>
-    <row r="2" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="66" t="s">
+    <row r="1" spans="1:2" s="27" customFormat="1" ht="69" customHeight="1">
+      <c r="A1" s="65" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="65"/>
+    </row>
+    <row r="2" spans="1:2" s="27" customFormat="1"/>
+    <row r="3" spans="1:2">
+      <c r="A3" s="55"/>
+      <c r="B3" s="57" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="27" customFormat="1">
+      <c r="A4" s="55"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="55"/>
+      <c r="B5" s="57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="27" customFormat="1">
+      <c r="A6" s="55"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="55"/>
+      <c r="B7" s="57" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="66" t="s">
+    <row r="8" spans="1:2" s="27" customFormat="1">
+      <c r="A8" s="55"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="55"/>
+      <c r="B9" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
-      <c r="B7" s="66" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="55"/>
+      <c r="B10" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
-      <c r="B9" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="55"/>
+      <c r="B11" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
-      <c r="B10" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="55"/>
+      <c r="B12" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
-      <c r="B11" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="55"/>
+      <c r="B13" s="58" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
-      <c r="B12" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="55"/>
+      <c r="B14" s="58" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
-      <c r="B13" s="67" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="55"/>
+      <c r="B15" s="58" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
-      <c r="B14" s="67" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="55"/>
+      <c r="B16" s="58" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
-      <c r="B15" s="67" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="55"/>
+      <c r="B17" s="58" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
-      <c r="B16" s="67" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="55"/>
+      <c r="B18" s="58" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
-      <c r="B17" s="67" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="55"/>
+      <c r="B19" s="58" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
-      <c r="B18" s="67" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="55"/>
+      <c r="B20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
-      <c r="B19" s="67" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="55"/>
+      <c r="B21" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
-      <c r="B20" t="s">
+    <row r="22" spans="1:2" s="27" customFormat="1">
+      <c r="A22" s="55"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="55"/>
+      <c r="B23" s="57" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
-      <c r="B21" t="s">
+    <row r="24" spans="1:2" s="27" customFormat="1">
+      <c r="A24" s="55"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="55"/>
+      <c r="B25" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
-      <c r="B23" s="66" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="55"/>
+      <c r="B26" s="58" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
-      <c r="B25" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="55"/>
+      <c r="B27" s="58" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
-      <c r="B26" s="67" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="55"/>
+      <c r="B28" s="58" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
-      <c r="B27" s="67" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="55"/>
+      <c r="B29" s="58" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="67" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="55"/>
+      <c r="B30" s="58" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="64"/>
-      <c r="B29" s="67" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="55"/>
+      <c r="B31" s="58" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="64"/>
-      <c r="B30" s="67" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="55"/>
+      <c r="B32" s="58" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
-      <c r="B31" s="67" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="55"/>
+      <c r="B33" s="58" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="64"/>
-      <c r="B32" s="67" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="55"/>
+      <c r="B34" s="58" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
-      <c r="B33" s="67" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="55"/>
+      <c r="B35" s="58" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="64"/>
-      <c r="B34" s="67" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="55"/>
+      <c r="B36" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="64"/>
-      <c r="B35" s="67" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="55"/>
+      <c r="B37" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
-      <c r="B36" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="55"/>
+      <c r="B38" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
-      <c r="B37" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="55"/>
+      <c r="B39" s="58" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="64"/>
-      <c r="B38" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="55"/>
+      <c r="B40" s="58" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="64"/>
-      <c r="B39" s="67" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="55"/>
+      <c r="B41" s="58" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="55"/>
+      <c r="B42" s="58" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="55"/>
+      <c r="B43" s="58" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="55"/>
+      <c r="B44" s="58" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="64"/>
-      <c r="B40" s="67" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="55"/>
+      <c r="B45" s="58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="55"/>
+      <c r="B46" s="58" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="55"/>
+      <c r="B47" s="58" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="55"/>
+      <c r="B48" s="58" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="64"/>
-      <c r="B41" s="67" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="64"/>
-      <c r="B42" s="67" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="64"/>
-      <c r="B43" s="67" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="64"/>
-      <c r="B44" s="67" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="55"/>
+      <c r="B49" s="58" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="64"/>
-      <c r="B45" s="67" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="64"/>
-      <c r="B46" s="67" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="64"/>
-      <c r="B47" s="67" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="64"/>
-      <c r="B48" s="67" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="55"/>
+      <c r="B50" s="58" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="64"/>
-      <c r="B49" s="67" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="55"/>
+      <c r="B51" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="64"/>
-      <c r="B50" s="67" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="55"/>
+      <c r="B52" s="58" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="64"/>
-      <c r="B51" s="67" t="s">
+    <row r="53" spans="1:2" s="27" customFormat="1"/>
+    <row r="54" spans="1:2">
+      <c r="A54" s="56"/>
+      <c r="B54" s="57" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="64"/>
-      <c r="B52" s="67" t="s">
+    <row r="55" spans="1:2" s="27" customFormat="1">
+      <c r="A55" s="56"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="56"/>
+      <c r="B56" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="65"/>
-      <c r="B54" s="66" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="56"/>
+      <c r="B57" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="65"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="65"/>
-      <c r="B56" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="56"/>
+      <c r="B58" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
-      <c r="B57" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="56"/>
+      <c r="B59" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="65"/>
-      <c r="B58" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="56"/>
+      <c r="B60" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
-      <c r="B59" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="56"/>
+      <c r="B61" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
-      <c r="B60" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="56"/>
+      <c r="B62" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="65"/>
-      <c r="B61" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="56"/>
+      <c r="B63" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
-      <c r="B62" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="56"/>
+      <c r="B64" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
-      <c r="B63" t="s">
+    <row r="65" spans="1:2" s="27" customFormat="1">
+      <c r="A65" s="56"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="56"/>
+      <c r="B66" s="57" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
-      <c r="B64" t="s">
+    <row r="67" spans="1:2" s="27" customFormat="1">
+      <c r="A67" s="56"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="56"/>
+      <c r="B68" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
-      <c r="B66" s="66" t="s">
+    <row r="69" spans="1:2" s="27" customFormat="1">
+      <c r="A69" s="56"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="56"/>
+      <c r="B70" s="57" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="65"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="65"/>
-      <c r="B68" t="s">
+    <row r="71" spans="1:2" s="27" customFormat="1">
+      <c r="A71" s="56"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="56"/>
+      <c r="B72" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
-      <c r="B70" s="66" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="56"/>
+      <c r="B73" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
-      <c r="B72" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="56"/>
+      <c r="B74" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="65"/>
-      <c r="B73" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="56"/>
+      <c r="B75" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="65"/>
-      <c r="B74" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="56"/>
+      <c r="B76" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="65"/>
-      <c r="B75" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="56"/>
+      <c r="B77" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
-      <c r="B76" t="s">
+    <row r="78" spans="1:2" s="27" customFormat="1">
+      <c r="A78" s="56"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="56"/>
+      <c r="B79" s="57" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
-      <c r="B77" t="s">
+    <row r="80" spans="1:2" s="27" customFormat="1">
+      <c r="A80" s="56"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="56"/>
+      <c r="B81" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
-      <c r="B79" s="66" t="s">
+    <row r="82" spans="1:2" s="27" customFormat="1">
+      <c r="A82" s="56"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="56"/>
+      <c r="B83" s="57" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="65"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="65"/>
-      <c r="B81" t="s">
+    <row r="84" spans="1:2" s="27" customFormat="1">
+      <c r="A84" s="56"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="56"/>
+      <c r="B85" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="65"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="65"/>
-      <c r="B83" s="66" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="56"/>
+      <c r="B86" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="65"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="65"/>
-      <c r="B85" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="56"/>
+      <c r="B87" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="65"/>
-      <c r="B86" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="65"/>
-      <c r="B87" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3778,14 +3741,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" style="19" customWidth="1"/>
     <col min="2" max="2" width="58" style="19" customWidth="1"/>
@@ -3794,170 +3757,170 @@
     <col min="5" max="5" width="58.140625" style="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="27" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+    <row r="1" spans="1:5" s="27" customFormat="1" ht="42.75" customHeight="1">
+      <c r="A1" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="52"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="44" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="154.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="D4" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="135.75" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" ht="140.25" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="51" t="s">
+      <c r="D6" s="49" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="49" t="s">
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="165">
+      <c r="A7" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="C7" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="193.5" customHeight="1">
+      <c r="A8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="60">
+      <c r="A9" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60">
+      <c r="A10" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="174" customHeight="1">
+      <c r="A11" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="C11" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="112.5" customHeight="1">
       <c r="A12" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="50" t="s">
         <v>181</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>182</v>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -3972,7 +3935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I236"/>
   <sheetViews>
@@ -3980,7 +3943,7 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.5703125" customWidth="1"/>
@@ -3993,20 +3956,20 @@
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:9" ht="18.75">
+      <c r="A1" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-    </row>
-    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+    </row>
+    <row r="2" spans="1:9" ht="31.5">
       <c r="A2" s="32"/>
       <c r="B2" s="39" t="s">
         <v>55</v>
@@ -4033,7 +3996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -4058,7 +4021,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="35"/>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -4083,7 +4046,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="35"/>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="25.5">
       <c r="A5" s="53">
         <v>3</v>
       </c>
@@ -4108,7 +4071,7 @@
       </c>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="53">
         <v>4</v>
       </c>
@@ -4131,7 +4094,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="35"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="53">
         <v>5</v>
       </c>
@@ -4156,7 +4119,7 @@
       </c>
       <c r="I7" s="35"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="25.5" hidden="1">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -4181,7 +4144,7 @@
       <c r="H8" s="30"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="25.5">
       <c r="A9" s="53">
         <v>7</v>
       </c>
@@ -4204,7 +4167,7 @@
       </c>
       <c r="I9" s="35"/>
     </row>
-    <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="38.25">
       <c r="A10" s="53">
         <v>8</v>
       </c>
@@ -4229,7 +4192,7 @@
       </c>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="25.5" hidden="1">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -4254,7 +4217,7 @@
       <c r="H11" s="30"/>
       <c r="I11" s="35"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1">
       <c r="A12" s="28">
         <v>10</v>
       </c>
@@ -4279,7 +4242,7 @@
       <c r="H12" s="30"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="53">
         <v>11</v>
       </c>
@@ -4306,7 +4269,7 @@
       </c>
       <c r="I13" s="35"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="53">
         <v>12</v>
       </c>
@@ -4331,7 +4294,7 @@
       <c r="H14" s="30"/>
       <c r="I14" s="35"/>
     </row>
-    <row r="15" spans="1:9" ht="153" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="153">
       <c r="A15" s="53">
         <v>13</v>
       </c>
@@ -4358,7 +4321,7 @@
       </c>
       <c r="I15" s="35"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -4379,7 +4342,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="35"/>
     </row>
-    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="38.25">
       <c r="A17" s="53">
         <v>15</v>
       </c>
@@ -4406,7 +4369,7 @@
       </c>
       <c r="I17" s="35"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="28"/>
       <c r="B18" s="34"/>
       <c r="C18" s="28"/>
@@ -4419,7 +4382,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="35"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="28"/>
       <c r="B19" s="34"/>
       <c r="C19" s="28"/>
@@ -4430,7 +4393,7 @@
       <c r="H19" s="30"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="28"/>
       <c r="B20" s="34"/>
       <c r="C20" s="28"/>
@@ -4441,7 +4404,7 @@
       <c r="H20" s="30"/>
       <c r="I20" s="35"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="28"/>
       <c r="B21" s="34"/>
       <c r="C21" s="28"/>
@@ -4452,7 +4415,7 @@
       <c r="H21" s="30"/>
       <c r="I21" s="35"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="28"/>
       <c r="B22" s="34"/>
       <c r="C22" s="28"/>
@@ -4463,7 +4426,7 @@
       <c r="H22" s="30"/>
       <c r="I22" s="35"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="28"/>
       <c r="B23" s="34"/>
       <c r="C23" s="28"/>
@@ -4474,7 +4437,7 @@
       <c r="H23" s="30"/>
       <c r="I23" s="35"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="28"/>
       <c r="B24" s="34"/>
       <c r="C24" s="28"/>
@@ -4485,7 +4448,7 @@
       <c r="H24" s="30"/>
       <c r="I24" s="35"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="28"/>
       <c r="B25" s="34"/>
       <c r="C25" s="28"/>
@@ -4496,7 +4459,7 @@
       <c r="H25" s="30"/>
       <c r="I25" s="35"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="28"/>
       <c r="B26" s="34"/>
       <c r="C26" s="28"/>
@@ -4507,7 +4470,7 @@
       <c r="H26" s="30"/>
       <c r="I26" s="35"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -4518,7 +4481,7 @@
       <c r="H27" s="27"/>
       <c r="I27" s="27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="27"/>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -4529,7 +4492,7 @@
       <c r="H28" s="27"/>
       <c r="I28" s="27"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="27"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -4540,7 +4503,7 @@
       <c r="H29" s="27"/>
       <c r="I29" s="27"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="27"/>
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
@@ -4551,7 +4514,7 @@
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="27"/>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -4562,7 +4525,7 @@
       <c r="H31" s="27"/>
       <c r="I31" s="27"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
@@ -4573,7 +4536,7 @@
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9">
       <c r="A225" s="27"/>
       <c r="B225" s="27"/>
       <c r="C225" s="27"/>
@@ -4584,7 +4547,7 @@
       <c r="H225" s="27"/>
       <c r="I225" s="27"/>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9">
       <c r="A226" s="27"/>
       <c r="B226" s="27"/>
       <c r="C226" s="27"/>
@@ -4595,7 +4558,7 @@
       <c r="H226" s="27"/>
       <c r="I226" s="27"/>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9">
       <c r="A227" s="27"/>
       <c r="B227" s="27"/>
       <c r="C227" s="27"/>
@@ -4606,7 +4569,7 @@
       <c r="H227" s="27"/>
       <c r="I227" s="27"/>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9">
       <c r="A228" s="27"/>
       <c r="B228" s="27"/>
       <c r="C228" s="27"/>
@@ -4617,7 +4580,7 @@
       <c r="H228" s="27"/>
       <c r="I228" s="27"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9">
       <c r="A229" s="27"/>
       <c r="B229" s="27"/>
       <c r="C229" s="27"/>
@@ -4628,7 +4591,7 @@
       <c r="H229" s="27"/>
       <c r="I229" s="27"/>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9">
       <c r="A230" s="27"/>
       <c r="B230" s="27"/>
       <c r="C230" s="27"/>
@@ -4639,7 +4602,7 @@
       <c r="H230" s="27"/>
       <c r="I230" s="27"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9">
       <c r="A231" s="27"/>
       <c r="B231" s="27"/>
       <c r="C231" s="27"/>
@@ -4650,7 +4613,7 @@
       <c r="H231" s="27"/>
       <c r="I231" s="27"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9">
       <c r="A232" s="27"/>
       <c r="B232" s="27"/>
       <c r="C232" s="27"/>
@@ -4661,7 +4624,7 @@
       <c r="H232" s="27"/>
       <c r="I232" s="27"/>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9">
       <c r="A233" s="27"/>
       <c r="B233" s="27"/>
       <c r="C233" s="27"/>
@@ -4672,7 +4635,7 @@
       <c r="H233" s="27"/>
       <c r="I233" s="27"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9">
       <c r="A234" s="27"/>
       <c r="B234" s="27"/>
       <c r="C234" s="27"/>
@@ -4683,7 +4646,7 @@
       <c r="H234" s="27"/>
       <c r="I234" s="27"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9">
       <c r="A235" s="27"/>
       <c r="B235" s="27"/>
       <c r="C235" s="27"/>
@@ -4694,7 +4657,7 @@
       <c r="H235" s="27"/>
       <c r="I235" s="27"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9">
       <c r="A236" s="27"/>
       <c r="B236" s="27"/>
       <c r="C236" s="27"/>
@@ -4706,7 +4669,7 @@
       <c r="I236" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I18" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A2:I18">
     <filterColumn colId="4">
       <filters blank="1">
         <dateGroupItem year="2018" month="6" dateTimeGrouping="month"/>
@@ -4716,7 +4679,7 @@
       </filters>
     </filterColumn>
     <filterColumn colId="5">
-      <filters blank="1">
+      <filters>
         <filter val="Homologação"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Data de atualização no documento
</commit_message>
<xml_diff>
--- a/Arquivos Externos/Controle CTI_QRD.xlsx
+++ b/Arquivos Externos/Controle CTI_QRD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorena\Documents\RGitRep\Arquivos Externos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165325D3-A642-4C29-8AEB-A62BF19D039F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36339FFF-6AFA-49A7-ACB3-6B47DEEEA8AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="20280" windowHeight="4725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2787,7 +2787,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
@@ -2849,7 +2849,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="7">
-        <v>43313</v>
+        <v>43333</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>

</xml_diff>

<commit_message>
Inclusão de item de clone de produção
</commit_message>
<xml_diff>
--- a/Arquivos Externos/Controle CTI_QRD.xlsx
+++ b/Arquivos Externos/Controle CTI_QRD.xlsx
@@ -23,14 +23,14 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId10"/>
-    <pivotCache cacheId="37" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="7" r:id="rId11"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2619" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="904">
   <si>
     <t>Item</t>
   </si>
@@ -4103,6 +4103,30 @@
 16/08/18 - Atualmente o flag de liminar foi extendido aos paineis de beneficiários, e uma solução utilizando a competência "-2"
 09/08/18 - Ação foi solicitada e contextualizada para equipe de BI QRD, novo cronograma deverá incluir item para seu acompanhamento
 24/07/18 - Citado em reunião, porém não foi atualizado no painel de pendências da equipe de BI</t>
+  </si>
+  <si>
+    <t>Ambiente deve estar consistente com produção para que testes de usuários possam ser realizados</t>
+  </si>
+  <si>
+    <t>Inconsistências em testes e impossibilidade de avaliar impactos</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30/08/18 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Verificar a frequencia de clonagem e a possibilidade de do fluxo: congelamentos em produção &gt; clonagem &gt; testes. Testes de regras foram seriamente comprometidos e usuários estão solicitando "testes em produção", prática não adequada</t>
+    </r>
+  </si>
+  <si>
+    <t>Clone de produção para homologação</t>
   </si>
 </sst>
 </file>
@@ -4766,7 +4790,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -5123,6 +5147,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -5456,7 +5483,7 @@
         <xdr:cNvPr id="1025" name="AutoShape 1" descr="Resultado de imagem para planserv">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5495,7 +5522,7 @@
         <xdr:cNvPr id="1027" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5546,7 +5573,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5592,7 +5619,7 @@
         <xdr:cNvPr id="2052" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5638,7 +5665,7 @@
         <xdr:cNvPr id="2054" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5684,7 +5711,7 @@
         <xdr:cNvPr id="2056" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5730,7 +5757,7 @@
         <xdr:cNvPr id="2058" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5776,7 +5803,7 @@
         <xdr:cNvPr id="2060" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5822,7 +5849,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5937,16 +5964,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Padrao2" refreshedDate="43341.446880787036" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="26">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Padrao2" refreshedDate="43342.428399999997" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="26">
   <cacheSource type="worksheet">
     <worksheetSource ref="A6:P32" sheet="Plano de ação"/>
   </cacheSource>
   <cacheFields count="16">
     <cacheField name="Prioridade" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="105"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="104"/>
     </cacheField>
     <cacheField name="ID" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="26"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="27"/>
     </cacheField>
     <cacheField name="Item" numFmtId="0">
       <sharedItems/>
@@ -5963,10 +5990,10 @@
         <s v="Geral"/>
         <s v="Regulação"/>
         <s v="Cadastro"/>
+        <s v="TI"/>
         <s v="Contas"/>
         <s v="Faturamento"/>
         <s v="Pagamento"/>
-        <s v="TI"/>
         <s v="Gestão"/>
         <s v="SLA"/>
       </sharedItems>
@@ -8246,10 +8273,28 @@
   </r>
   <r>
     <n v="5"/>
+    <n v="27"/>
+    <s v="Clone de produção para homologação"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="Ambiente deve estar consistente com produção para que testes de usuários possam ser realizados"/>
+    <s v="Item novo"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Inconsistências em testes e impossibilidade de avaliar impactos"/>
+    <m/>
+    <s v="Nelson"/>
+    <s v="Bernardo"/>
+    <d v="2018-08-30T00:00:00"/>
+    <s v="30/08/18 - Verificar a frequencia de clonagem e a possibilidade de do fluxo: congelamentos em produção &gt; clonagem &gt; testes. Testes de regras foram seriamente comprometidos e usuários estão solicitando &quot;testes em produção&quot;, prática não adequada"/>
+    <m/>
+  </r>
+  <r>
+    <n v="6"/>
     <n v="25"/>
     <s v="Integração TISS"/>
     <x v="1"/>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Acompanhamento das ações que regularizaram o XML de retorno de contas para prestadores"/>
     <s v="Item novo"/>
     <x v="3"/>
@@ -8263,7 +8308,7 @@
     <m/>
   </r>
   <r>
-    <n v="6"/>
+    <n v="7"/>
     <n v="14"/>
     <s v="Relatório de Governo"/>
     <x v="0"/>
@@ -8281,11 +8326,11 @@
     <m/>
   </r>
   <r>
-    <n v="7"/>
+    <n v="8"/>
     <n v="23"/>
     <s v="CONSIG"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Funcionalidades que permitam manutenção de todas as interações com orgãos do estado (outros poderes e executivo), com geração de arquivos para consignação "/>
     <s v="Em acompanhamento"/>
     <x v="1"/>
@@ -8299,7 +8344,7 @@
     <m/>
   </r>
   <r>
-    <n v="8"/>
+    <n v="9"/>
     <n v="24"/>
     <s v="Cadastro Online"/>
     <x v="1"/>
@@ -8317,11 +8362,11 @@
     <m/>
   </r>
   <r>
-    <n v="9"/>
+    <n v="10"/>
     <n v="13"/>
     <s v="Dados de pagamento"/>
     <x v="1"/>
-    <x v="5"/>
+    <x v="6"/>
     <s v="Relatório Glosa de Edital Março a Junho de 2018"/>
     <s v="Relatório para CG, sem atendimento desde criação em 18/07/18"/>
     <x v="2"/>
@@ -8335,11 +8380,11 @@
     <m/>
   </r>
   <r>
-    <n v="10"/>
+    <n v="11"/>
     <n v="18"/>
     <s v="Liminar no painel de contas"/>
     <x v="0"/>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Marcação de liminar ainda não foi associada da solicitação para respectiva conta"/>
     <s v="Comunicada"/>
     <x v="1"/>
@@ -8353,11 +8398,11 @@
     <m/>
   </r>
   <r>
-    <n v="11"/>
+    <n v="12"/>
     <n v="1"/>
     <s v="Modelo de dados - Stage 1"/>
     <x v="0"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Diagrama da base de dados intermediária, com dados relacionados às áreas de negócio"/>
     <s v="Em avaliação"/>
     <x v="1"/>
@@ -8371,7 +8416,7 @@
     <m/>
   </r>
   <r>
-    <n v="12"/>
+    <n v="13"/>
     <n v="19"/>
     <s v="Nomeclatura em paineis do BI"/>
     <x v="0"/>
@@ -8389,7 +8434,7 @@
     <m/>
   </r>
   <r>
-    <n v="13"/>
+    <n v="14"/>
     <n v="26"/>
     <s v="SMS para autorizações"/>
     <x v="1"/>
@@ -8407,11 +8452,11 @@
     <m/>
   </r>
   <r>
-    <n v="14"/>
+    <n v="15"/>
     <n v="17"/>
     <s v="Pedidos de acesso"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Controle realizados por e-mail não estão funcionando bem, o Jira deve ser utilizado com acordo referente a prazos"/>
     <s v="Em avaliação"/>
     <x v="4"/>
@@ -8425,11 +8470,11 @@
     <m/>
   </r>
   <r>
-    <n v="15"/>
+    <n v="16"/>
     <n v="7"/>
     <s v="Release Notes para mudanças do BI"/>
     <x v="0"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Padrão de notas sobre alterações realizadas no modelo"/>
     <s v="Em avaliação"/>
     <x v="4"/>
@@ -8501,7 +8546,7 @@
     <n v="11"/>
     <s v="Recebimento automático de chamados"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Resposta automatizada no Jira impede aferição correta da primeira resposta dada por um técnico ao avaliar chamados abertos"/>
     <s v="Realizar acompanhamento mensal"/>
     <x v="5"/>
@@ -8573,7 +8618,7 @@
     <n v="20"/>
     <s v="Atualização de dados da Cópia_STG 1"/>
     <x v="0"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Assegurar que dados da base com acesso pelo Planserv estão atualizados a D-1"/>
     <s v="Resolvida"/>
     <x v="6"/>
@@ -8591,7 +8636,7 @@
     <n v="2"/>
     <s v="Acesso à Stage 1 - VPN"/>
     <x v="1"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Proposta de acesso à base de dados de negócio para equipe TI PSV"/>
     <s v="Resolvida"/>
     <x v="6"/>
@@ -8609,7 +8654,7 @@
     <n v="5"/>
     <s v="Área de protótipo para criação de paineis"/>
     <x v="0"/>
-    <x v="6"/>
+    <x v="3"/>
     <s v="Espaço com dados limitados, em ambiente de homologação, permitindo salvamento das visões no Power BI"/>
     <s v="Resolvida"/>
     <x v="6"/>
@@ -8620,31 +8665,13 @@
     <s v="Raniere"/>
     <s v="AD"/>
     <s v="01/08/18 - Foi liberado 30/07/18 será avaliado pela equipe.&#10;&#10;27/01/18 - PRevisão de entrega somente em 17/08, será feito novo alinamento em 31/07 para entendimento das dificuldades técnicas.&#10;&#10;06/07/18 - Foi realizada tentativa de envio do arquivo como alternativa ao acesso web pelo módulo analítico, sem sucesso&#10;&#10;04/07/18 - Formalizado por André Machado em resumo sobre reuniões realizadas em 03 e 04/07. Foi sinalizado por Raniere necessidade de intervenção da TI QRD para que o painel fosse disponibilizado, com previsão de produção na semana de 09 a 13/07, porém entrega ainda não foi realizada até o momento."/>
-    <m/>
-  </r>
-  <r>
-    <n v="105"/>
-    <n v="10"/>
-    <s v="Mudanças de status indevidas no Jira"/>
-    <x v="1"/>
-    <x v="6"/>
-    <s v="Comentários informativos pela TI QRD estão ocasionando mudanças para status &quot;aguardando solicitante&quot; e gerando paradas de relógio indevidas para os chamados"/>
-    <s v="Resolvida"/>
-    <x v="6"/>
-    <x v="1"/>
-    <s v="Apuração correta do tempo de atendimento"/>
-    <m/>
-    <s v="Nelson"/>
-    <s v="André Duarte/Denis"/>
-    <s v="AD"/>
-    <s v="03/08/18 - Removida a automação que muda o status do chamado quando o atendente comenta. A alteração será manual.&#10;&#10;01/08/18 - Será mudado no fluxo Jira, com mudança para &quot;Aguardando solicitante&quot; somente quando a função validar for executada pela equipe de suporte QRD&#10;&#10;24/07/18 - Tratado em reunião com André Machado e Denis, será avaliado para novas ocorrências"/>
     <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A5:I22" firstHeaderRow="0" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -8661,14 +8688,14 @@
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
       <items count="9">
         <item x="2"/>
-        <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
         <item x="0"/>
         <item x="7"/>
-        <item x="5"/>
+        <item x="6"/>
         <item x="1"/>
         <item x="8"/>
-        <item x="6"/>
+        <item x="3"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
@@ -9009,7 +9036,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica5" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -9395,7 +9422,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -9476,7 +9502,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="7">
-        <v>43341</v>
+        <v>43342</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -9661,7 +9687,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="119.25" customHeight="1">
-      <c r="A9" s="6">
+      <c r="A9" s="105">
         <v>3</v>
       </c>
       <c r="B9" s="6">
@@ -9773,23 +9799,23 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="102.75" customHeight="1">
-      <c r="A11" s="6">
+      <c r="A11" s="105">
         <v>5</v>
       </c>
       <c r="B11" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>314</v>
+        <v>903</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>424</v>
+        <v>18</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>315</v>
+        <v>900</v>
       </c>
       <c r="G11" s="90" t="s">
         <v>261</v>
@@ -9801,7 +9827,7 @@
         <v>417</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>316</v>
+        <v>901</v>
       </c>
       <c r="K11" s="14"/>
       <c r="L11" s="6" t="s">
@@ -9814,7 +9840,7 @@
         <v>43342</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="P11" s="9"/>
       <c r="R11" s="13" t="s">
@@ -9829,46 +9855,44 @@
         <v>6</v>
       </c>
       <c r="B12" s="6">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>400</v>
+        <v>314</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="G12" s="90" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>407</v>
+        <v>261</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>410</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>399</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="K12" s="14"/>
       <c r="L12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>305</v>
+        <v>105</v>
       </c>
       <c r="N12" s="22">
         <v>43342</v>
       </c>
-      <c r="O12" s="35" t="s">
-        <v>403</v>
+      <c r="O12" s="9" t="s">
+        <v>897</v>
       </c>
       <c r="P12" s="9"/>
       <c r="R12" s="15" t="s">
@@ -9879,48 +9903,50 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="98.25" customHeight="1">
-      <c r="A13" s="6">
+      <c r="A13" s="105">
         <v>7</v>
       </c>
       <c r="B13" s="6">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G13" s="90" t="s">
-        <v>395</v>
+        <v>113</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>407</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="K13" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>399</v>
+      </c>
       <c r="L13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>105</v>
+        <v>305</v>
       </c>
       <c r="N13" s="110">
         <v>43342</v>
       </c>
-      <c r="O13" s="9" t="s">
-        <v>892</v>
+      <c r="O13" s="35" t="s">
+        <v>403</v>
       </c>
       <c r="P13" s="9"/>
       <c r="R13" s="64" t="s">
@@ -9935,46 +9961,44 @@
         <v>8</v>
       </c>
       <c r="B14" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>401</v>
+        <v>300</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>260</v>
+        <v>301</v>
       </c>
       <c r="G14" s="90" t="s">
-        <v>394</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>408</v>
+        <v>395</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>407</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>417</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>398</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="K14" s="14"/>
       <c r="L14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>313</v>
+        <v>105</v>
       </c>
       <c r="N14" s="110">
         <v>43342</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="P14" s="9"/>
       <c r="U14" s="14" t="s">
@@ -9982,26 +10006,26 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="109.5" customHeight="1">
-      <c r="A15" s="6">
+      <c r="A15" s="105">
         <v>9</v>
       </c>
       <c r="B15" s="6">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
       <c r="G15" s="90" t="s">
-        <v>100</v>
+        <v>394</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>408</v>
@@ -10010,22 +10034,22 @@
         <v>417</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>101</v>
+        <v>262</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>98</v>
+        <v>398</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="N15" s="110">
         <v>43342</v>
       </c>
-      <c r="O15" s="35" t="s">
-        <v>894</v>
+      <c r="O15" s="9" t="s">
+        <v>893</v>
       </c>
       <c r="P15" s="9"/>
       <c r="U15" s="14" t="s">
@@ -10037,44 +10061,46 @@
         <v>10</v>
       </c>
       <c r="B16" s="6">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>19</v>
-      </c>
       <c r="E16" s="14" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="G16" s="90" t="s">
-        <v>161</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>407</v>
+        <v>100</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>408</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="K16" s="14"/>
+        <v>101</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="L16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="N16" s="22">
         <v>43342</v>
       </c>
-      <c r="O16" s="9" t="s">
-        <v>899</v>
+      <c r="O16" s="35" t="s">
+        <v>894</v>
       </c>
       <c r="P16" s="9"/>
       <c r="U16" s="14" t="s">
@@ -10082,26 +10108,26 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="153" customHeight="1">
-      <c r="A17" s="6">
+      <c r="A17" s="105">
         <v>11</v>
       </c>
       <c r="B17" s="6">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>18</v>
+        <v>424</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>9</v>
+        <v>145</v>
       </c>
       <c r="G17" s="90" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="H17" s="16" t="s">
         <v>407</v>
@@ -10110,7 +10136,7 @@
         <v>418</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="K17" s="14"/>
       <c r="L17" s="6" t="s">
@@ -10123,7 +10149,7 @@
         <v>43342</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>404</v>
+        <v>899</v>
       </c>
       <c r="P17" s="9"/>
       <c r="U17" s="14" t="s">
@@ -10135,31 +10161,31 @@
         <v>12</v>
       </c>
       <c r="B18" s="6">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>421</v>
+        <v>18</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G18" s="118" t="s">
-        <v>889</v>
-      </c>
-      <c r="H18" s="64" t="s">
-        <v>331</v>
+        <v>9</v>
+      </c>
+      <c r="G18" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>407</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>418</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="K18" s="14"/>
       <c r="L18" s="6" t="s">
@@ -10172,126 +10198,126 @@
         <v>43342</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>895</v>
+        <v>404</v>
       </c>
       <c r="P18" s="9"/>
       <c r="U18" s="14" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="105">
-      <c r="A19" s="6">
+    <row r="19" spans="1:21" ht="330">
+      <c r="A19" s="105">
         <v>13</v>
       </c>
       <c r="B19" s="6">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>317</v>
+        <v>148</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="G19" s="90" t="s">
-        <v>261</v>
-      </c>
-      <c r="H19" s="65" t="s">
-        <v>410</v>
+        <v>149</v>
+      </c>
+      <c r="G19" s="118" t="s">
+        <v>889</v>
+      </c>
+      <c r="H19" s="64" t="s">
+        <v>331</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>418</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>319</v>
+        <v>150</v>
       </c>
       <c r="K19" s="14"/>
       <c r="L19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="N19" s="22">
         <v>43342</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>312</v>
+        <v>895</v>
       </c>
       <c r="P19" s="9"/>
       <c r="U19" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="141.75" hidden="1" customHeight="1">
+    <row r="20" spans="1:21" ht="141.75" customHeight="1">
       <c r="A20" s="6">
         <v>14</v>
       </c>
       <c r="B20" s="6">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>114</v>
+        <v>317</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>18</v>
+        <v>422</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>115</v>
+        <v>318</v>
       </c>
       <c r="G20" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" s="64" t="s">
-        <v>331</v>
+        <v>261</v>
+      </c>
+      <c r="H20" s="65" t="s">
+        <v>410</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>418</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>116</v>
+        <v>319</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="N20" s="39" t="s">
-        <v>147</v>
+        <v>105</v>
+      </c>
+      <c r="N20" s="22">
+        <v>43342</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="P20" s="9"/>
     </row>
-    <row r="21" spans="1:21" ht="158.25" hidden="1" customHeight="1">
-      <c r="A21" s="6">
+    <row r="21" spans="1:21" ht="158.25" customHeight="1">
+      <c r="A21" s="105">
         <v>15</v>
       </c>
       <c r="B21" s="6">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="G21" s="90" t="s">
         <v>97</v>
@@ -10303,124 +10329,124 @@
         <v>418</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="N21" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>396</v>
+        <v>306</v>
       </c>
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="1:21" ht="135.75" customHeight="1">
       <c r="A22" s="6">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B22" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>427</v>
+        <v>18</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="G22" s="90" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="63" t="s">
-        <v>411</v>
+        <v>97</v>
+      </c>
+      <c r="H22" s="64" t="s">
+        <v>331</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>418</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="K22" s="14"/>
       <c r="L22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="N22" s="22">
-        <v>43342</v>
+        <v>21</v>
+      </c>
+      <c r="N22" s="39" t="s">
+        <v>147</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>896</v>
+        <v>396</v>
       </c>
       <c r="P22" s="9"/>
     </row>
-    <row r="23" spans="1:21" ht="97.5" hidden="1" customHeight="1">
+    <row r="23" spans="1:21" ht="97.5" customHeight="1">
       <c r="A23" s="6">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="6">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="G23" s="90" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="H23" s="63" t="s">
         <v>411</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="N23" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="O23" s="35" t="s">
-        <v>164</v>
+        <v>26</v>
+      </c>
+      <c r="N23" s="22">
+        <v>43342</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>896</v>
       </c>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:21" ht="123" hidden="1" customHeight="1">
+    <row r="24" spans="1:21" ht="123" customHeight="1">
       <c r="A24" s="6">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>18</v>
@@ -10441,41 +10467,41 @@
         <v>419</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K24" s="14"/>
       <c r="L24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M24" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N24" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O24" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P24" s="9"/>
     </row>
-    <row r="25" spans="1:21" ht="140.25" hidden="1" customHeight="1">
+    <row r="25" spans="1:21" ht="140.25" customHeight="1">
       <c r="A25" s="6">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="6">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>18</v>
+        <v>422</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="G25" s="90" t="s">
         <v>103</v>
@@ -10484,44 +10510,44 @@
         <v>411</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="K25" s="14"/>
       <c r="L25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M25" s="14" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="N25" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="O25" s="9" t="s">
-        <v>117</v>
+      <c r="O25" s="35" t="s">
+        <v>165</v>
       </c>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="1:21" ht="87" hidden="1" customHeight="1">
+    <row r="26" spans="1:21" ht="87" customHeight="1">
       <c r="A26" s="6">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>428</v>
+        <v>18</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="G26" s="90" t="s">
         <v>103</v>
@@ -10533,32 +10559,32 @@
         <v>418</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="M26" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="N26" s="33" t="s">
-        <v>31</v>
+        <v>93</v>
+      </c>
+      <c r="N26" s="39" t="s">
+        <v>147</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="P26" s="9"/>
     </row>
-    <row r="27" spans="1:21" ht="87.75" hidden="1" customHeight="1">
+    <row r="27" spans="1:21" ht="87.75" customHeight="1">
       <c r="A27" s="6">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>19</v>
@@ -10567,7 +10593,7 @@
         <v>428</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G27" s="90" t="s">
         <v>103</v>
@@ -10596,70 +10622,70 @@
       </c>
       <c r="P27" s="9"/>
     </row>
-    <row r="28" spans="1:21" ht="100.5" hidden="1" customHeight="1">
+    <row r="28" spans="1:21" ht="100.5" customHeight="1">
       <c r="A28" s="6">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="B28" s="6">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>428</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="G28" s="90" t="s">
-        <v>163</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>163</v>
+        <v>103</v>
+      </c>
+      <c r="H28" s="63" t="s">
+        <v>411</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>418</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="K28" s="14"/>
       <c r="L28" s="6" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="N28" s="39" t="s">
-        <v>147</v>
+        <v>30</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P28" s="9"/>
     </row>
-    <row r="29" spans="1:21" ht="97.5" hidden="1" customHeight="1">
+    <row r="29" spans="1:21" ht="97.5" customHeight="1">
       <c r="A29" s="6">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="6">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>234</v>
+        <v>94</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>18</v>
+        <v>428</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="G29" s="90" t="s">
         <v>163</v>
@@ -10668,44 +10694,44 @@
         <v>163</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="K29" s="14"/>
       <c r="L29" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M29" s="14" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="N29" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>253</v>
+        <v>162</v>
       </c>
       <c r="P29" s="9"/>
     </row>
-    <row r="30" spans="1:21" ht="112.5" hidden="1" customHeight="1">
+    <row r="30" spans="1:21" ht="112.5" customHeight="1">
       <c r="A30" s="6">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>303</v>
+        <v>234</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="G30" s="90" t="s">
         <v>163</v>
@@ -10717,41 +10743,41 @@
         <v>417</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="K30" s="14"/>
       <c r="L30" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M30" s="14" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="N30" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="P30" s="9"/>
     </row>
-    <row r="31" spans="1:21" ht="138" hidden="1" customHeight="1">
+    <row r="31" spans="1:21" ht="138" customHeight="1">
       <c r="A31" s="6">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>39</v>
+        <v>303</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G31" s="90" t="s">
         <v>163</v>
@@ -10763,41 +10789,41 @@
         <v>417</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K31" s="14"/>
       <c r="L31" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M31" s="14" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="N31" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="P31" s="9"/>
     </row>
-    <row r="32" spans="1:21" ht="110.25" hidden="1" customHeight="1">
+    <row r="32" spans="1:21" ht="110.25" customHeight="1">
       <c r="A32" s="6">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="G32" s="90" t="s">
         <v>163</v>
@@ -10806,47 +10832,73 @@
         <v>163</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="K32" s="14"/>
       <c r="L32" s="6" t="s">
         <v>10</v>
       </c>
       <c r="M32" s="14" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="N32" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O32" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="P32" s="9"/>
+    </row>
+    <row r="33" spans="1:16" ht="150">
+      <c r="A33" s="6">
+        <v>105</v>
+      </c>
+      <c r="B33" s="6">
+        <v>10</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="90" t="s">
+        <v>163</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="N33" s="131" t="s">
+        <v>147</v>
+      </c>
+      <c r="O33" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="P32" s="9"/>
-    </row>
-    <row r="33" spans="1:16" hidden="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6">
-        <v>27</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
-    <row r="34" spans="1:16" hidden="1">
+    <row r="34" spans="1:16">
       <c r="A34" s="6"/>
       <c r="B34" s="6">
         <v>28</v>
@@ -10866,7 +10918,7 @@
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
-    <row r="35" spans="1:16" hidden="1">
+    <row r="35" spans="1:16">
       <c r="A35" s="6"/>
       <c r="B35" s="6">
         <v>29</v>
@@ -10886,7 +10938,7 @@
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
-    <row r="36" spans="1:16" hidden="1">
+    <row r="36" spans="1:16">
       <c r="A36" s="6"/>
       <c r="B36" s="6">
         <v>30</v>
@@ -10906,7 +10958,7 @@
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
-    <row r="37" spans="1:16" hidden="1">
+    <row r="37" spans="1:16">
       <c r="A37" s="6"/>
       <c r="B37" s="6">
         <v>31</v>
@@ -10926,7 +10978,7 @@
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
     </row>
-    <row r="38" spans="1:16" hidden="1">
+    <row r="38" spans="1:16">
       <c r="A38" s="6"/>
       <c r="B38" s="6">
         <v>32</v>
@@ -10946,7 +10998,7 @@
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
-    <row r="39" spans="1:16" hidden="1">
+    <row r="39" spans="1:16">
       <c r="A39" s="6"/>
       <c r="B39" s="6">
         <v>33</v>
@@ -10966,7 +11018,7 @@
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
-    <row r="40" spans="1:16" hidden="1">
+    <row r="40" spans="1:16">
       <c r="A40" s="6"/>
       <c r="B40" s="6">
         <v>34</v>
@@ -10986,7 +11038,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="9"/>
     </row>
-    <row r="41" spans="1:16" hidden="1">
+    <row r="41" spans="1:16">
       <c r="A41" s="6"/>
       <c r="B41" s="6">
         <v>35</v>
@@ -11006,7 +11058,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
     </row>
-    <row r="42" spans="1:16" hidden="1">
+    <row r="42" spans="1:16">
       <c r="A42" s="6"/>
       <c r="B42" s="6">
         <v>36</v>
@@ -11026,7 +11078,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
     </row>
-    <row r="43" spans="1:16" hidden="1">
+    <row r="43" spans="1:16">
       <c r="A43" s="6"/>
       <c r="B43" s="6">
         <v>37</v>
@@ -11046,7 +11098,7 @@
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
     </row>
-    <row r="44" spans="1:16" hidden="1">
+    <row r="44" spans="1:16">
       <c r="A44" s="6"/>
       <c r="B44" s="6">
         <v>38</v>
@@ -11066,7 +11118,7 @@
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
     </row>
-    <row r="45" spans="1:16" hidden="1">
+    <row r="45" spans="1:16">
       <c r="A45" s="6"/>
       <c r="B45" s="6">
         <v>39</v>
@@ -11086,7 +11138,7 @@
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
     </row>
-    <row r="46" spans="1:16" hidden="1">
+    <row r="46" spans="1:16">
       <c r="A46" s="6"/>
       <c r="B46" s="6">
         <v>40</v>
@@ -11106,7 +11158,7 @@
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
     </row>
-    <row r="47" spans="1:16" hidden="1">
+    <row r="47" spans="1:16">
       <c r="A47" s="6"/>
       <c r="B47" s="6">
         <v>41</v>
@@ -11126,7 +11178,7 @@
       <c r="O47" s="9"/>
       <c r="P47" s="9"/>
     </row>
-    <row r="48" spans="1:16" hidden="1">
+    <row r="48" spans="1:16">
       <c r="A48" s="6"/>
       <c r="B48" s="6">
         <v>42</v>
@@ -11146,7 +11198,7 @@
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>
     </row>
-    <row r="49" spans="1:16" hidden="1">
+    <row r="49" spans="1:16">
       <c r="A49" s="6"/>
       <c r="B49" s="6">
         <v>43</v>
@@ -11166,7 +11218,7 @@
       <c r="O49" s="9"/>
       <c r="P49" s="9"/>
     </row>
-    <row r="50" spans="1:16" hidden="1">
+    <row r="50" spans="1:16">
       <c r="A50" s="6"/>
       <c r="B50" s="6">
         <v>44</v>
@@ -11186,7 +11238,7 @@
       <c r="O50" s="9"/>
       <c r="P50" s="9"/>
     </row>
-    <row r="51" spans="1:16" hidden="1">
+    <row r="51" spans="1:16">
       <c r="A51" s="6"/>
       <c r="B51" s="6">
         <v>45</v>
@@ -11206,7 +11258,7 @@
       <c r="O51" s="9"/>
       <c r="P51" s="9"/>
     </row>
-    <row r="52" spans="1:16" hidden="1">
+    <row r="52" spans="1:16">
       <c r="A52" s="6"/>
       <c r="B52" s="6">
         <v>46</v>
@@ -11226,7 +11278,7 @@
       <c r="O52" s="9"/>
       <c r="P52" s="9"/>
     </row>
-    <row r="53" spans="1:16" hidden="1">
+    <row r="53" spans="1:16">
       <c r="A53" s="6"/>
       <c r="B53" s="6">
         <v>47</v>
@@ -11246,7 +11298,7 @@
       <c r="O53" s="9"/>
       <c r="P53" s="9"/>
     </row>
-    <row r="54" spans="1:16" hidden="1">
+    <row r="54" spans="1:16">
       <c r="A54" s="6"/>
       <c r="B54" s="6">
         <v>48</v>
@@ -11266,7 +11318,7 @@
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
     </row>
-    <row r="55" spans="1:16" hidden="1">
+    <row r="55" spans="1:16">
       <c r="A55" s="6"/>
       <c r="B55" s="6">
         <v>49</v>
@@ -11286,7 +11338,7 @@
       <c r="O55" s="9"/>
       <c r="P55" s="9"/>
     </row>
-    <row r="56" spans="1:16" hidden="1">
+    <row r="56" spans="1:16">
       <c r="A56" s="6"/>
       <c r="B56" s="6">
         <v>50</v>
@@ -11306,7 +11358,7 @@
       <c r="O56" s="9"/>
       <c r="P56" s="9"/>
     </row>
-    <row r="57" spans="1:16" hidden="1">
+    <row r="57" spans="1:16">
       <c r="A57" s="6"/>
       <c r="B57" s="6">
         <v>51</v>
@@ -11326,7 +11378,7 @@
       <c r="O57" s="9"/>
       <c r="P57" s="9"/>
     </row>
-    <row r="58" spans="1:16" hidden="1">
+    <row r="58" spans="1:16">
       <c r="A58" s="6"/>
       <c r="B58" s="6">
         <v>52</v>
@@ -11346,7 +11398,7 @@
       <c r="O58" s="9"/>
       <c r="P58" s="9"/>
     </row>
-    <row r="59" spans="1:16" hidden="1">
+    <row r="59" spans="1:16">
       <c r="A59" s="6"/>
       <c r="B59" s="6">
         <v>53</v>
@@ -11366,7 +11418,7 @@
       <c r="O59" s="9"/>
       <c r="P59" s="9"/>
     </row>
-    <row r="60" spans="1:16" hidden="1">
+    <row r="60" spans="1:16">
       <c r="A60" s="6"/>
       <c r="B60" s="6">
         <v>54</v>
@@ -11386,7 +11438,7 @@
       <c r="O60" s="9"/>
       <c r="P60" s="9"/>
     </row>
-    <row r="61" spans="1:16" hidden="1">
+    <row r="61" spans="1:16">
       <c r="A61" s="6"/>
       <c r="B61" s="6">
         <v>55</v>
@@ -11406,7 +11458,7 @@
       <c r="O61" s="9"/>
       <c r="P61" s="9"/>
     </row>
-    <row r="62" spans="1:16" hidden="1">
+    <row r="62" spans="1:16">
       <c r="A62" s="6"/>
       <c r="B62" s="6">
         <v>56</v>
@@ -11426,7 +11478,7 @@
       <c r="O62" s="9"/>
       <c r="P62" s="9"/>
     </row>
-    <row r="63" spans="1:16" hidden="1">
+    <row r="63" spans="1:16">
       <c r="A63" s="6"/>
       <c r="B63" s="6">
         <v>57</v>
@@ -11446,7 +11498,7 @@
       <c r="O63" s="9"/>
       <c r="P63" s="9"/>
     </row>
-    <row r="64" spans="1:16" hidden="1">
+    <row r="64" spans="1:16">
       <c r="A64" s="6"/>
       <c r="B64" s="6">
         <v>58</v>
@@ -11466,7 +11518,7 @@
       <c r="O64" s="9"/>
       <c r="P64" s="9"/>
     </row>
-    <row r="65" spans="1:16" hidden="1">
+    <row r="65" spans="1:16">
       <c r="A65" s="6"/>
       <c r="B65" s="6">
         <v>59</v>
@@ -11486,7 +11538,7 @@
       <c r="O65" s="9"/>
       <c r="P65" s="9"/>
     </row>
-    <row r="66" spans="1:16" hidden="1">
+    <row r="66" spans="1:16">
       <c r="A66" s="6"/>
       <c r="B66" s="6">
         <v>60</v>
@@ -11510,13 +11562,9 @@
   <autoFilter ref="A6:P66">
     <filterColumn colId="4"/>
     <filterColumn colId="7"/>
-    <filterColumn colId="13">
-      <filters>
-        <dateGroupItem year="2018" dateTimeGrouping="year"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="13"/>
     <sortState ref="A7:P66">
-      <sortCondition ref="A6:A38"/>
+      <sortCondition ref="A6:A66"/>
     </sortState>
   </autoFilter>
   <sortState ref="U7:U19">
@@ -14712,7 +14760,7 @@
   <dimension ref="A3:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14782,13 +14830,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="96">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D7" s="94">
         <v>7</v>
       </c>
       <c r="E7" s="96">
-        <v>0.33333333333333331</v>
+        <v>0.31818181818181818</v>
       </c>
       <c r="F7" s="94"/>
       <c r="G7" s="96">
@@ -14798,7 +14846,7 @@
         <v>8</v>
       </c>
       <c r="I7" s="96">
-        <v>0.38095238095238093</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -14813,7 +14861,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="F8" s="92"/>
       <c r="G8" s="95">
@@ -14823,7 +14871,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -14834,13 +14882,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D9" s="92">
         <v>2</v>
       </c>
       <c r="E9" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="F9" s="92"/>
       <c r="G9" s="95">
@@ -14850,7 +14898,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="95">
-        <v>0.14285714285714285</v>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -14865,7 +14913,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="F10" s="92"/>
       <c r="G10" s="95">
@@ -14875,7 +14923,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -14890,7 +14938,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="F11" s="92"/>
       <c r="G11" s="95">
@@ -14900,7 +14948,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -14908,28 +14956,28 @@
         <v>18</v>
       </c>
       <c r="B12" s="94">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="96">
-        <v>0.2857142857142857</v>
+        <v>0.31818181818181818</v>
       </c>
       <c r="D12" s="94">
         <v>3</v>
       </c>
       <c r="E12" s="96">
-        <v>0.14285714285714285</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="F12" s="94">
         <v>2</v>
       </c>
       <c r="G12" s="96">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="H12" s="94">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" s="96">
-        <v>0.52380952380952384</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -14940,7 +14988,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="D13" s="92"/>
       <c r="E13" s="95">
@@ -14954,7 +15002,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -14965,7 +15013,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D14" s="92"/>
       <c r="E14" s="95">
@@ -14979,7 +15027,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -14990,7 +15038,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D15" s="92"/>
       <c r="E15" s="95">
@@ -15004,7 +15052,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -15015,7 +15063,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D16" s="92"/>
       <c r="E16" s="95">
@@ -15029,7 +15077,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -15040,50 +15088,52 @@
         <v>1</v>
       </c>
       <c r="C17" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D17" s="92">
         <v>1</v>
       </c>
       <c r="E17" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="F17" s="92">
         <v>2</v>
       </c>
       <c r="G17" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="H17" s="92">
         <v>4</v>
       </c>
       <c r="I17" s="95">
-        <v>0.19047619047619047</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="92"/>
+      <c r="B18" s="92">
+        <v>1</v>
+      </c>
       <c r="C18" s="95">
-        <v>0</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D18" s="92">
         <v>2</v>
       </c>
       <c r="E18" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="F18" s="92"/>
       <c r="G18" s="95">
         <v>0</v>
       </c>
       <c r="H18" s="92">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>0.13636363636363635</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -15094,13 +15144,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="96">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D19" s="94">
         <v>1</v>
       </c>
       <c r="E19" s="96">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="F19" s="94"/>
       <c r="G19" s="96">
@@ -15110,7 +15160,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="96">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -15121,7 +15171,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D20" s="92"/>
       <c r="E20" s="95">
@@ -15135,7 +15185,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -15150,7 +15200,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="F21" s="92"/>
       <c r="G21" s="95">
@@ -15160,7 +15210,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="95">
-        <v>4.7619047619047616E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -15168,25 +15218,25 @@
         <v>412</v>
       </c>
       <c r="B22" s="92">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="95">
-        <v>0.38095238095238093</v>
+        <v>0.40909090909090912</v>
       </c>
       <c r="D22" s="92">
         <v>11</v>
       </c>
       <c r="E22" s="95">
-        <v>0.52380952380952384</v>
+        <v>0.5</v>
       </c>
       <c r="F22" s="92">
         <v>2</v>
       </c>
       <c r="G22" s="95">
-        <v>9.5238095238095233E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="H22" s="92">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I22" s="95">
         <v>1</v>

</xml_diff>